<commit_message>
actions, change in templates
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/exemption_request/001_Exemption_Request.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/exemption_request/001_Exemption_Request.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aot\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\eao\beta\code\epictrack-api\src\api\templates\event_templates\exemption_request\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E238C48D-FD6D-42D5-828D-D07C0DDD7593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E25389-8E21-435D-BE5D-E40194146CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="Events" sheetId="3" r:id="rId3"/>
     <sheet name="Outcomes" sheetId="4" r:id="rId4"/>
     <sheet name="Actions" sheetId="6" r:id="rId5"/>
-    <sheet name="Lookups" sheetId="2" r:id="rId6"/>
+    <sheet name="ActionBackup" sheetId="7" r:id="rId6"/>
+    <sheet name="Lookups" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="271">
   <si>
     <t>No</t>
   </si>
@@ -949,6 +950,84 @@
   </si>
   <si>
     <t>Create a new WORK: "EAC Assessment" and link to thisWorkLinkedProject</t>
+  </si>
+  <si>
+    <t>Visibility</t>
+  </si>
+  <si>
+    <t>REGULAR</t>
+  </si>
+  <si>
+    <t>MANDATORY</t>
+  </si>
+  <si>
+    <t>OPTIONAL</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Exemption Early Engagement","work_type_id": 5, "ea_act_id": 3, "event_name": "Approval of IPD/EP Submission", "start_at": 1 }</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Exemption Request Intake","work_type_id": 5, "ea_act_id": 3, "event_name": "Submission of "Draft" Initial Project Description &amp; Engagement Plan", "start_at": 21 }</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Exemption Request Intake","work_type_id": 5, "ea_act_id": 3, "event_name": "\"Draft\" Initial Project Description &amp; Engagement Plan Initial Review", "start_at": 28 }</t>
+  </si>
+  <si>
+    <t>{"all_future_phases":false}</t>
+  </si>
+  <si>
+    <t>{"work_state": "WITHDRAWN"}</t>
+  </si>
+  <si>
+    <t>{"is_active": false}</t>
+  </si>
+  <si>
+    <t>{"start_date_locked": true}</t>
+  </si>
+  <si>
+    <t>{"work_type":15}</t>
+  </si>
+  <si>
+    <t>{"work_state": "TERMINATED"}</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Exemption DPD Development (Proponent Time)","work_type_id": 5, "ea_act_id": 3, "event_name": "Start of DPD Development (Proponent Time) (Date Capture Milestone)", "start_at": 1}</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Exemption Readiness Decision","work_type_id": 5, "ea_act_id": 3, "event_name": "Detailed Project Description Received", "start_at": 1}</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Exemption DPD Development (Proponent Time)","work_type_id": 5, "ea_act_id": 3, "event_name": "Submission of \"Draft\" Detailed Project Description", "start_at": 21 }</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Exemption DPD Development (Proponent Time)","work_type_id": 5, "ea_act_id": 3, "event_name": "\"Draft\" Detailed Project Description Initial Review", "start_at": 28 }</t>
+  </si>
+  <si>
+    <t>HIDDEN</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Exemption Readiness Decision","work_type_id": 5, "ea_act_id": 3, "event_name": "Decision: Readiness Decision" }</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Exemption DPD Development (Proponent Time)","work_type_id": 5, "ea_act_id": 3, "new_name": "Exemption DPD Development (Proponent Time)", "legislated": false }</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Exemption Readiness Decision","work_type_id": 5, "ea_act_id": 3, "new_name": "Exemption Readiness Decision", "legislated": false }</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Exemption DPD Development (Proponent Time)","work_type_id": 5, "ea_act_id": 3, "event_name": "Start of DPD Development (Proponent Time) (Date Capture Milestone)", "start_at": 1 }</t>
+  </si>
+  <si>
+    <t>Set workState to COMPLETED</t>
+  </si>
+  <si>
+    <t>{"work_state": "COMPLETED"}</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Further Readiness Decision","work_type_id": 5, "ea_act_id": 3, "new_name": "Further Readiness Decision", "legislated": false }</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Further Readiness Decision","work_type_id": 5, "ea_act_id": 3, "event_name": "Readiness Decision Report referred to CEAO for Further Decision", "start_at": 1}</t>
   </si>
 </sst>
 </file>
@@ -1602,13 +1681,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8789B1A8-4095-496B-ABDA-23EBF7B52DFC}">
-  <dimension ref="A1:H156"/>
+  <dimension ref="A1:I156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1617,12 +1696,12 @@
     <col min="2" max="2" width="50.77734375" style="2" customWidth="1"/>
     <col min="3" max="3" width="24.77734375" style="2" customWidth="1"/>
     <col min="4" max="5" width="14.77734375" style="2" customWidth="1"/>
-    <col min="6" max="7" width="12.77734375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.77734375" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="2"/>
+    <col min="6" max="8" width="12.77734375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1645,10 +1724,13 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1670,11 +1752,14 @@
       <c r="G2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="I2" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1696,11 +1781,14 @@
       <c r="G3" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="I3" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1722,11 +1810,14 @@
       <c r="G4" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="I4" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1748,11 +1839,14 @@
       <c r="G5" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="I5" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1774,11 +1868,14 @@
       <c r="G6" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="I6" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1800,35 +1897,38 @@
       <c r="G7" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="I7" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
@@ -2285,10 +2385,10 @@
   <dimension ref="A1:N126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F77" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F53" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E103" sqref="E103"/>
+      <selection pane="bottomRight" activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2301,8 +2401,7 @@
     <col min="7" max="7" width="32.77734375" style="2" customWidth="1"/>
     <col min="8" max="10" width="14.77734375" style="2" customWidth="1"/>
     <col min="11" max="11" width="18.77734375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="14.77734375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="12.77734375" style="2" customWidth="1"/>
+    <col min="12" max="13" width="14.77734375" style="2" customWidth="1"/>
     <col min="14" max="14" width="10.77734375" style="2" customWidth="1"/>
     <col min="15" max="16384" width="8.88671875" style="2"/>
   </cols>
@@ -2342,7 +2441,7 @@
         <v>4</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>31</v>
+        <v>245</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>7</v>
@@ -2380,8 +2479,8 @@
       <c r="L2" s="3">
         <v>0</v>
       </c>
-      <c r="M2" s="8" t="b">
-        <v>1</v>
+      <c r="M2" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N2" s="3">
         <v>1</v>
@@ -2419,8 +2518,8 @@
       <c r="L3" s="3">
         <v>0</v>
       </c>
-      <c r="M3" s="8" t="b">
-        <v>1</v>
+      <c r="M3" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N3" s="3">
         <v>2</v>
@@ -2458,8 +2557,8 @@
       <c r="L4" s="3">
         <v>0</v>
       </c>
-      <c r="M4" s="8" t="b">
-        <v>1</v>
+      <c r="M4" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N4" s="3">
         <v>3</v>
@@ -2500,8 +2599,8 @@
       <c r="L5" s="3">
         <v>0</v>
       </c>
-      <c r="M5" s="8" t="b">
-        <v>1</v>
+      <c r="M5" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N5" s="3">
         <v>4</v>
@@ -2539,8 +2638,8 @@
       <c r="L6" s="3">
         <v>0</v>
       </c>
-      <c r="M6" s="8" t="b">
-        <v>1</v>
+      <c r="M6" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N6" s="3">
         <v>5</v>
@@ -2578,8 +2677,8 @@
       <c r="L7" s="3">
         <v>0</v>
       </c>
-      <c r="M7" s="8" t="b">
-        <v>1</v>
+      <c r="M7" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N7" s="3">
         <v>6</v>
@@ -2620,8 +2719,8 @@
       <c r="L8" s="3">
         <v>0</v>
       </c>
-      <c r="M8" s="8" t="b">
-        <v>1</v>
+      <c r="M8" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N8" s="3">
         <v>7</v>
@@ -2662,8 +2761,8 @@
       <c r="L9" s="3">
         <v>0</v>
       </c>
-      <c r="M9" s="8" t="b">
-        <v>1</v>
+      <c r="M9" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N9" s="3">
         <v>8</v>
@@ -2701,8 +2800,8 @@
       <c r="L10" s="3">
         <v>0</v>
       </c>
-      <c r="M10" s="8" t="b">
-        <v>0</v>
+      <c r="M10" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N10" s="3">
         <v>9</v>
@@ -2743,8 +2842,8 @@
       <c r="L11" s="3">
         <v>0</v>
       </c>
-      <c r="M11" s="8" t="b">
-        <v>0</v>
+      <c r="M11" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N11" s="3">
         <v>10</v>
@@ -2782,8 +2881,8 @@
       <c r="L12" s="3">
         <v>0</v>
       </c>
-      <c r="M12" s="8" t="b">
-        <v>0</v>
+      <c r="M12" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N12" s="3">
         <v>11</v>
@@ -2821,8 +2920,8 @@
       <c r="L13" s="3">
         <v>0</v>
       </c>
-      <c r="M13" s="8" t="b">
-        <v>1</v>
+      <c r="M13" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N13" s="3">
         <v>12</v>
@@ -2863,8 +2962,8 @@
       <c r="L14" s="3">
         <v>0</v>
       </c>
-      <c r="M14" s="8" t="b">
-        <v>1</v>
+      <c r="M14" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N14" s="3">
         <v>13</v>
@@ -2905,8 +3004,8 @@
       <c r="L15" s="3">
         <v>0</v>
       </c>
-      <c r="M15" s="8" t="b">
-        <v>1</v>
+      <c r="M15" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N15" s="3">
         <v>14</v>
@@ -2947,8 +3046,8 @@
       <c r="L16" s="3">
         <v>0</v>
       </c>
-      <c r="M16" s="8" t="b">
-        <v>1</v>
+      <c r="M16" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N16" s="3">
         <v>15</v>
@@ -2986,8 +3085,8 @@
       <c r="L17" s="3">
         <v>0</v>
       </c>
-      <c r="M17" s="8" t="b">
-        <v>1</v>
+      <c r="M17" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N17" s="3">
         <v>16</v>
@@ -3025,8 +3124,8 @@
       <c r="L18" s="3">
         <v>30</v>
       </c>
-      <c r="M18" s="8" t="b">
-        <v>1</v>
+      <c r="M18" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N18" s="3">
         <v>17</v>
@@ -3067,8 +3166,8 @@
       <c r="L19" s="3">
         <v>0</v>
       </c>
-      <c r="M19" s="8" t="b">
-        <v>1</v>
+      <c r="M19" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N19" s="3">
         <v>18</v>
@@ -3109,8 +3208,8 @@
       <c r="L20" s="3">
         <v>0</v>
       </c>
-      <c r="M20" s="8" t="b">
-        <v>1</v>
+      <c r="M20" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N20" s="3">
         <v>19</v>
@@ -3151,8 +3250,8 @@
       <c r="L21" s="3">
         <v>0</v>
       </c>
-      <c r="M21" s="8" t="b">
-        <v>1</v>
+      <c r="M21" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N21" s="3">
         <v>20</v>
@@ -3193,8 +3292,8 @@
       <c r="L22" s="3">
         <v>0</v>
       </c>
-      <c r="M22" s="8" t="b">
-        <v>1</v>
+      <c r="M22" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N22" s="3">
         <v>21</v>
@@ -3232,8 +3331,8 @@
       <c r="L23" s="3">
         <v>0</v>
       </c>
-      <c r="M23" s="8" t="b">
-        <v>1</v>
+      <c r="M23" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N23" s="3">
         <v>22</v>
@@ -3274,8 +3373,8 @@
       <c r="L24" s="3">
         <v>0</v>
       </c>
-      <c r="M24" s="8" t="b">
-        <v>1</v>
+      <c r="M24" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N24" s="3">
         <v>23</v>
@@ -3313,8 +3412,8 @@
       <c r="L25" s="3">
         <v>0</v>
       </c>
-      <c r="M25" s="8" t="b">
-        <v>1</v>
+      <c r="M25" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N25" s="3">
         <v>24</v>
@@ -3355,8 +3454,8 @@
       <c r="L26" s="3">
         <v>0</v>
       </c>
-      <c r="M26" s="8" t="b">
-        <v>1</v>
+      <c r="M26" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N26" s="3">
         <v>25</v>
@@ -3394,8 +3493,8 @@
       <c r="L27" s="3">
         <v>0</v>
       </c>
-      <c r="M27" s="8" t="b">
-        <v>1</v>
+      <c r="M27" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N27" s="3">
         <v>26</v>
@@ -3433,8 +3532,8 @@
       <c r="L28" s="3">
         <v>0</v>
       </c>
-      <c r="M28" s="8" t="b">
-        <v>1</v>
+      <c r="M28" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N28" s="3">
         <v>27</v>
@@ -3475,8 +3574,8 @@
       <c r="L29" s="3">
         <v>0</v>
       </c>
-      <c r="M29" s="8" t="b">
-        <v>1</v>
+      <c r="M29" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N29" s="3">
         <v>28</v>
@@ -3514,8 +3613,8 @@
       <c r="L30" s="3">
         <v>0</v>
       </c>
-      <c r="M30" s="8" t="b">
-        <v>0</v>
+      <c r="M30" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N30" s="3">
         <v>29</v>
@@ -3553,8 +3652,8 @@
       <c r="L31" s="3">
         <v>0</v>
       </c>
-      <c r="M31" s="8" t="b">
-        <v>0</v>
+      <c r="M31" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N31" s="3">
         <v>30</v>
@@ -3595,8 +3694,8 @@
       <c r="L32" s="3">
         <v>0</v>
       </c>
-      <c r="M32" s="8" t="b">
-        <v>0</v>
+      <c r="M32" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N32" s="3">
         <v>31</v>
@@ -3637,8 +3736,8 @@
       <c r="L33" s="3">
         <v>0</v>
       </c>
-      <c r="M33" s="8" t="b">
-        <v>0</v>
+      <c r="M33" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N33" s="3">
         <v>32</v>
@@ -3679,8 +3778,8 @@
       <c r="L34" s="3">
         <v>0</v>
       </c>
-      <c r="M34" s="8" t="b">
-        <v>0</v>
+      <c r="M34" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N34" s="3">
         <v>33</v>
@@ -3721,8 +3820,8 @@
       <c r="L35" s="3">
         <v>0</v>
       </c>
-      <c r="M35" s="8" t="b">
-        <v>0</v>
+      <c r="M35" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N35" s="3">
         <v>34</v>
@@ -3760,8 +3859,8 @@
       <c r="L36" s="3">
         <v>30</v>
       </c>
-      <c r="M36" s="8" t="b">
-        <v>0</v>
+      <c r="M36" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N36" s="3">
         <v>35</v>
@@ -3802,8 +3901,8 @@
       <c r="L37" s="3">
         <v>0</v>
       </c>
-      <c r="M37" s="8" t="b">
-        <v>0</v>
+      <c r="M37" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N37" s="3">
         <v>36</v>
@@ -3844,8 +3943,8 @@
       <c r="L38" s="3">
         <v>0</v>
       </c>
-      <c r="M38" s="8" t="b">
-        <v>0</v>
+      <c r="M38" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N38" s="3">
         <v>37</v>
@@ -3886,8 +3985,8 @@
       <c r="L39" s="3">
         <v>0</v>
       </c>
-      <c r="M39" s="8" t="b">
-        <v>0</v>
+      <c r="M39" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N39" s="3">
         <v>38</v>
@@ -3928,8 +4027,8 @@
       <c r="L40" s="3">
         <v>0</v>
       </c>
-      <c r="M40" s="8" t="b">
-        <v>0</v>
+      <c r="M40" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N40" s="3">
         <v>39</v>
@@ -3967,8 +4066,8 @@
       <c r="L41" s="3">
         <v>0</v>
       </c>
-      <c r="M41" s="8" t="b">
-        <v>0</v>
+      <c r="M41" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N41" s="3">
         <v>40</v>
@@ -4006,8 +4105,8 @@
       <c r="L42" s="3">
         <v>0</v>
       </c>
-      <c r="M42" s="8" t="b">
-        <v>0</v>
+      <c r="M42" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N42" s="3">
         <v>41</v>
@@ -4045,8 +4144,8 @@
       <c r="L43" s="3">
         <v>0</v>
       </c>
-      <c r="M43" s="8" t="b">
-        <v>0</v>
+      <c r="M43" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N43" s="3">
         <v>42</v>
@@ -4087,8 +4186,8 @@
       <c r="L44" s="3">
         <v>0</v>
       </c>
-      <c r="M44" s="8" t="b">
-        <v>0</v>
+      <c r="M44" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N44" s="3">
         <v>43</v>
@@ -4129,8 +4228,8 @@
       <c r="L45" s="3">
         <v>0</v>
       </c>
-      <c r="M45" s="8" t="b">
-        <v>0</v>
+      <c r="M45" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N45" s="3">
         <v>44</v>
@@ -4168,8 +4267,8 @@
       <c r="L46" s="3">
         <v>0</v>
       </c>
-      <c r="M46" s="8" t="b">
-        <v>0</v>
+      <c r="M46" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N46" s="3">
         <v>45</v>
@@ -4210,8 +4309,8 @@
       <c r="L47" s="3">
         <v>0</v>
       </c>
-      <c r="M47" s="8" t="b">
-        <v>0</v>
+      <c r="M47" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N47" s="3">
         <v>46</v>
@@ -4252,8 +4351,8 @@
       <c r="L48" s="3">
         <v>0</v>
       </c>
-      <c r="M48" s="8" t="b">
-        <v>0</v>
+      <c r="M48" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N48" s="3">
         <v>47</v>
@@ -4291,8 +4390,8 @@
       <c r="L49" s="3">
         <v>0</v>
       </c>
-      <c r="M49" s="8" t="b">
-        <v>0</v>
+      <c r="M49" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N49" s="3">
         <v>48</v>
@@ -4333,8 +4432,8 @@
       <c r="L50" s="3">
         <v>0</v>
       </c>
-      <c r="M50" s="8" t="b">
-        <v>0</v>
+      <c r="M50" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N50" s="3">
         <v>49</v>
@@ -4375,8 +4474,8 @@
       <c r="L51" s="3">
         <v>0</v>
       </c>
-      <c r="M51" s="8" t="b">
-        <v>0</v>
+      <c r="M51" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N51" s="3">
         <v>50</v>
@@ -4414,8 +4513,8 @@
       <c r="L52" s="3">
         <v>0</v>
       </c>
-      <c r="M52" s="8" t="b">
-        <v>0</v>
+      <c r="M52" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N52" s="3">
         <v>51</v>
@@ -4456,8 +4555,8 @@
       <c r="L53" s="3">
         <v>0</v>
       </c>
-      <c r="M53" s="8" t="b">
-        <v>0</v>
+      <c r="M53" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N53" s="3">
         <v>52</v>
@@ -4498,8 +4597,8 @@
       <c r="L54" s="3">
         <v>0</v>
       </c>
-      <c r="M54" s="8" t="b">
-        <v>0</v>
+      <c r="M54" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N54" s="3">
         <v>53</v>
@@ -4540,8 +4639,8 @@
       <c r="L55" s="3">
         <v>0</v>
       </c>
-      <c r="M55" s="8" t="b">
-        <v>0</v>
+      <c r="M55" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N55" s="3">
         <v>54</v>
@@ -4582,8 +4681,8 @@
       <c r="L56" s="3">
         <v>0</v>
       </c>
-      <c r="M56" s="8" t="b">
-        <v>0</v>
+      <c r="M56" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N56" s="3">
         <v>55</v>
@@ -4624,8 +4723,8 @@
       <c r="L57" s="3">
         <v>0</v>
       </c>
-      <c r="M57" s="8" t="b">
-        <v>0</v>
+      <c r="M57" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N57" s="3">
         <v>56</v>
@@ -4666,8 +4765,8 @@
       <c r="L58" s="3">
         <v>0</v>
       </c>
-      <c r="M58" s="8" t="b">
-        <v>0</v>
+      <c r="M58" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N58" s="3">
         <v>57</v>
@@ -4708,8 +4807,8 @@
       <c r="L59" s="3">
         <v>0</v>
       </c>
-      <c r="M59" s="8" t="b">
-        <v>0</v>
+      <c r="M59" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N59" s="3">
         <v>58</v>
@@ -4750,8 +4849,8 @@
       <c r="L60" s="3">
         <v>0</v>
       </c>
-      <c r="M60" s="8" t="b">
-        <v>0</v>
+      <c r="M60" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N60" s="3">
         <v>59</v>
@@ -4789,8 +4888,8 @@
       <c r="L61" s="3">
         <v>0</v>
       </c>
-      <c r="M61" s="8" t="b">
-        <v>0</v>
+      <c r="M61" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N61" s="3">
         <v>60</v>
@@ -4831,8 +4930,8 @@
       <c r="L62" s="3">
         <v>0</v>
       </c>
-      <c r="M62" s="8" t="b">
-        <v>1</v>
+      <c r="M62" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N62" s="3">
         <v>61</v>
@@ -4873,8 +4972,8 @@
       <c r="L63" s="3">
         <v>0</v>
       </c>
-      <c r="M63" s="8" t="b">
-        <v>1</v>
+      <c r="M63" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N63" s="3">
         <v>62</v>
@@ -4915,8 +5014,8 @@
       <c r="L64" s="3">
         <v>0</v>
       </c>
-      <c r="M64" s="8" t="b">
-        <v>1</v>
+      <c r="M64" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N64" s="3">
         <v>63</v>
@@ -4954,8 +5053,8 @@
       <c r="L65" s="3">
         <v>0</v>
       </c>
-      <c r="M65" s="8" t="b">
-        <v>1</v>
+      <c r="M65" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N65" s="3">
         <v>64</v>
@@ -4993,8 +5092,8 @@
       <c r="L66" s="3">
         <v>0</v>
       </c>
-      <c r="M66" s="8" t="b">
-        <v>1</v>
+      <c r="M66" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N66" s="3">
         <v>65</v>
@@ -5032,8 +5131,8 @@
       <c r="L67" s="3">
         <v>0</v>
       </c>
-      <c r="M67" s="8" t="b">
-        <v>1</v>
+      <c r="M67" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N67" s="3">
         <v>66</v>
@@ -5074,8 +5173,8 @@
       <c r="L68" s="3">
         <v>0</v>
       </c>
-      <c r="M68" s="8" t="b">
-        <v>1</v>
+      <c r="M68" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N68" s="3">
         <v>67</v>
@@ -5116,8 +5215,8 @@
       <c r="L69" s="3">
         <v>0</v>
       </c>
-      <c r="M69" s="8" t="b">
-        <v>1</v>
+      <c r="M69" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N69" s="3">
         <v>68</v>
@@ -5155,8 +5254,8 @@
       <c r="L70" s="3">
         <v>0</v>
       </c>
-      <c r="M70" s="8" t="b">
-        <v>0</v>
+      <c r="M70" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N70" s="3">
         <v>69</v>
@@ -5197,8 +5296,8 @@
       <c r="L71" s="3">
         <v>0</v>
       </c>
-      <c r="M71" s="8" t="b">
-        <v>0</v>
+      <c r="M71" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N71" s="3">
         <v>70</v>
@@ -5239,8 +5338,8 @@
       <c r="L72" s="3">
         <v>0</v>
       </c>
-      <c r="M72" s="8" t="b">
-        <v>0</v>
+      <c r="M72" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N72" s="3">
         <v>71</v>
@@ -5281,8 +5380,8 @@
       <c r="L73" s="3">
         <v>0</v>
       </c>
-      <c r="M73" s="8" t="b">
-        <v>0</v>
+      <c r="M73" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N73" s="3">
         <v>72</v>
@@ -5323,8 +5422,8 @@
       <c r="L74" s="3">
         <v>0</v>
       </c>
-      <c r="M74" s="8" t="b">
-        <v>0</v>
+      <c r="M74" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N74" s="3">
         <v>73</v>
@@ -5365,8 +5464,8 @@
       <c r="L75" s="3">
         <v>0</v>
       </c>
-      <c r="M75" s="8" t="b">
-        <v>0</v>
+      <c r="M75" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N75" s="3">
         <v>74</v>
@@ -5407,8 +5506,8 @@
       <c r="L76" s="3">
         <v>0</v>
       </c>
-      <c r="M76" s="8" t="b">
-        <v>0</v>
+      <c r="M76" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N76" s="3">
         <v>75</v>
@@ -5449,8 +5548,8 @@
       <c r="L77" s="3">
         <v>0</v>
       </c>
-      <c r="M77" s="8" t="b">
-        <v>0</v>
+      <c r="M77" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N77" s="3">
         <v>76</v>
@@ -5491,8 +5590,8 @@
       <c r="L78" s="3">
         <v>0</v>
       </c>
-      <c r="M78" s="8" t="b">
-        <v>0</v>
+      <c r="M78" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N78" s="3">
         <v>77</v>
@@ -5533,8 +5632,8 @@
       <c r="L79" s="3">
         <v>0</v>
       </c>
-      <c r="M79" s="8" t="b">
-        <v>0</v>
+      <c r="M79" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N79" s="3">
         <v>78</v>
@@ -5572,8 +5671,8 @@
       <c r="L80" s="3">
         <v>0</v>
       </c>
-      <c r="M80" s="8" t="b">
-        <v>0</v>
+      <c r="M80" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N80" s="3">
         <v>79</v>
@@ -5611,8 +5710,8 @@
       <c r="L81" s="3">
         <v>0</v>
       </c>
-      <c r="M81" s="8" t="b">
-        <v>1</v>
+      <c r="M81" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N81" s="3">
         <v>80</v>
@@ -5650,8 +5749,8 @@
       <c r="L82" s="3">
         <v>0</v>
       </c>
-      <c r="M82" s="8" t="b">
-        <v>1</v>
+      <c r="M82" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N82" s="3">
         <v>81</v>
@@ -5692,8 +5791,8 @@
       <c r="L83" s="3">
         <v>0</v>
       </c>
-      <c r="M83" s="8" t="b">
-        <v>1</v>
+      <c r="M83" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N83" s="3">
         <v>82</v>
@@ -5734,8 +5833,8 @@
       <c r="L84" s="3">
         <v>0</v>
       </c>
-      <c r="M84" s="8" t="b">
-        <v>1</v>
+      <c r="M84" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N84" s="3">
         <v>83</v>
@@ -5773,8 +5872,8 @@
       <c r="L85" s="3">
         <v>0</v>
       </c>
-      <c r="M85" s="8" t="b">
-        <v>1</v>
+      <c r="M85" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N85" s="3">
         <v>84</v>
@@ -5812,8 +5911,8 @@
       <c r="L86" s="3">
         <v>0</v>
       </c>
-      <c r="M86" s="8" t="b">
-        <v>1</v>
+      <c r="M86" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N86" s="3">
         <v>85</v>
@@ -5854,8 +5953,8 @@
       <c r="L87" s="3">
         <v>0</v>
       </c>
-      <c r="M87" s="8" t="b">
-        <v>1</v>
+      <c r="M87" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N87" s="3">
         <v>86</v>
@@ -5896,8 +5995,8 @@
       <c r="L88" s="3">
         <v>0</v>
       </c>
-      <c r="M88" s="8" t="b">
-        <v>1</v>
+      <c r="M88" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N88" s="3">
         <v>87</v>
@@ -5938,8 +6037,8 @@
       <c r="L89" s="3">
         <v>0</v>
       </c>
-      <c r="M89" s="8" t="b">
-        <v>1</v>
+      <c r="M89" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N89" s="3">
         <v>88</v>
@@ -5980,8 +6079,8 @@
       <c r="L90" s="3">
         <v>0</v>
       </c>
-      <c r="M90" s="8" t="b">
-        <v>1</v>
+      <c r="M90" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N90" s="3">
         <v>89</v>
@@ -6019,8 +6118,8 @@
       <c r="L91" s="3">
         <v>0</v>
       </c>
-      <c r="M91" s="8" t="b">
-        <v>1</v>
+      <c r="M91" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N91" s="3">
         <v>90</v>
@@ -6058,8 +6157,8 @@
       <c r="L92" s="3">
         <v>0</v>
       </c>
-      <c r="M92" s="8" t="b">
-        <v>0</v>
+      <c r="M92" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N92" s="3">
         <v>91</v>
@@ -6100,8 +6199,8 @@
       <c r="L93" s="3">
         <v>0</v>
       </c>
-      <c r="M93" s="8" t="b">
-        <v>0</v>
+      <c r="M93" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N93" s="3">
         <v>92</v>
@@ -6142,8 +6241,8 @@
       <c r="L94" s="3">
         <v>0</v>
       </c>
-      <c r="M94" s="8" t="b">
-        <v>0</v>
+      <c r="M94" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N94" s="3">
         <v>93</v>
@@ -6184,8 +6283,8 @@
       <c r="L95" s="3">
         <v>0</v>
       </c>
-      <c r="M95" s="8" t="b">
-        <v>0</v>
+      <c r="M95" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N95" s="3">
         <v>94</v>
@@ -6226,8 +6325,8 @@
       <c r="L96" s="3">
         <v>0</v>
       </c>
-      <c r="M96" s="8" t="b">
-        <v>0</v>
+      <c r="M96" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N96" s="3">
         <v>95</v>
@@ -6268,8 +6367,8 @@
       <c r="L97" s="3">
         <v>0</v>
       </c>
-      <c r="M97" s="8" t="b">
-        <v>0</v>
+      <c r="M97" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N97" s="3">
         <v>96</v>
@@ -6310,8 +6409,8 @@
       <c r="L98" s="3">
         <v>0</v>
       </c>
-      <c r="M98" s="8" t="b">
-        <v>0</v>
+      <c r="M98" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N98" s="3">
         <v>97</v>
@@ -6352,8 +6451,8 @@
       <c r="L99" s="3">
         <v>0</v>
       </c>
-      <c r="M99" s="8" t="b">
-        <v>0</v>
+      <c r="M99" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N99" s="3">
         <v>98</v>
@@ -6394,8 +6493,8 @@
       <c r="L100" s="3">
         <v>0</v>
       </c>
-      <c r="M100" s="8" t="b">
-        <v>0</v>
+      <c r="M100" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N100" s="3">
         <v>99</v>
@@ -6436,8 +6535,8 @@
       <c r="L101" s="3">
         <v>0</v>
       </c>
-      <c r="M101" s="8" t="b">
-        <v>0</v>
+      <c r="M101" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N101" s="3">
         <v>100</v>
@@ -6475,8 +6574,8 @@
       <c r="L102" s="3">
         <v>0</v>
       </c>
-      <c r="M102" s="8" t="b">
-        <v>0</v>
+      <c r="M102" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N102" s="3">
         <v>101</v>
@@ -6514,8 +6613,8 @@
       <c r="L103" s="3">
         <v>0</v>
       </c>
-      <c r="M103" s="8" t="b">
-        <v>1</v>
+      <c r="M103" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N103" s="3">
         <v>102</v>
@@ -6553,8 +6652,8 @@
       <c r="L104" s="3">
         <v>0</v>
       </c>
-      <c r="M104" s="8" t="b">
-        <v>1</v>
+      <c r="M104" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N104" s="3">
         <v>103</v>
@@ -6592,8 +6691,8 @@
       <c r="L105" s="3">
         <v>0</v>
       </c>
-      <c r="M105" s="8" t="b">
-        <v>0</v>
+      <c r="M105" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N105" s="3">
         <v>104</v>
@@ -6634,8 +6733,8 @@
       <c r="L106" s="3">
         <v>0</v>
       </c>
-      <c r="M106" s="8" t="b">
-        <v>0</v>
+      <c r="M106" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N106" s="3">
         <v>105</v>
@@ -6676,8 +6775,8 @@
       <c r="L107" s="3">
         <v>0</v>
       </c>
-      <c r="M107" s="8" t="b">
-        <v>0</v>
+      <c r="M107" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N107" s="3">
         <v>106</v>
@@ -6718,8 +6817,8 @@
       <c r="L108" s="3">
         <v>0</v>
       </c>
-      <c r="M108" s="8" t="b">
-        <v>0</v>
+      <c r="M108" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N108" s="3">
         <v>107</v>
@@ -6760,8 +6859,8 @@
       <c r="L109" s="3">
         <v>0</v>
       </c>
-      <c r="M109" s="8" t="b">
-        <v>0</v>
+      <c r="M109" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N109" s="3">
         <v>108</v>
@@ -6802,8 +6901,8 @@
       <c r="L110" s="3">
         <v>0</v>
       </c>
-      <c r="M110" s="8" t="b">
-        <v>0</v>
+      <c r="M110" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N110" s="3">
         <v>109</v>
@@ -6844,8 +6943,8 @@
       <c r="L111" s="3">
         <v>0</v>
       </c>
-      <c r="M111" s="8" t="b">
-        <v>0</v>
+      <c r="M111" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N111" s="3">
         <v>110</v>
@@ -6883,8 +6982,8 @@
       <c r="L112" s="3">
         <v>0</v>
       </c>
-      <c r="M112" s="8" t="b">
-        <v>0</v>
+      <c r="M112" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N112" s="3">
         <v>111</v>
@@ -6925,8 +7024,8 @@
       <c r="L113" s="3">
         <v>0</v>
       </c>
-      <c r="M113" s="8" t="b">
-        <v>1</v>
+      <c r="M113" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N113" s="3">
         <v>112</v>
@@ -6967,8 +7066,8 @@
       <c r="L114" s="3">
         <v>0</v>
       </c>
-      <c r="M114" s="8" t="b">
-        <v>1</v>
+      <c r="M114" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N114" s="3">
         <v>113</v>
@@ -7006,8 +7105,8 @@
       <c r="L115" s="3">
         <v>0</v>
       </c>
-      <c r="M115" s="8" t="b">
-        <v>1</v>
+      <c r="M115" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N115" s="3">
         <v>114</v>
@@ -7045,8 +7144,8 @@
       <c r="L116" s="3">
         <v>0</v>
       </c>
-      <c r="M116" s="8" t="b">
-        <v>0</v>
+      <c r="M116" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N116" s="3">
         <v>115</v>
@@ -7087,8 +7186,8 @@
       <c r="L117" s="3">
         <v>0</v>
       </c>
-      <c r="M117" s="8" t="b">
-        <v>0</v>
+      <c r="M117" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N117" s="3">
         <v>116</v>
@@ -7129,8 +7228,8 @@
       <c r="L118" s="3">
         <v>0</v>
       </c>
-      <c r="M118" s="8" t="b">
-        <v>0</v>
+      <c r="M118" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N118" s="3">
         <v>117</v>
@@ -7171,8 +7270,8 @@
       <c r="L119" s="3">
         <v>0</v>
       </c>
-      <c r="M119" s="8" t="b">
-        <v>0</v>
+      <c r="M119" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N119" s="3">
         <v>118</v>
@@ -7213,8 +7312,8 @@
       <c r="L120" s="3">
         <v>0</v>
       </c>
-      <c r="M120" s="8" t="b">
-        <v>0</v>
+      <c r="M120" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N120" s="3">
         <v>119</v>
@@ -7255,8 +7354,8 @@
       <c r="L121" s="3">
         <v>0</v>
       </c>
-      <c r="M121" s="8" t="b">
-        <v>0</v>
+      <c r="M121" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N121" s="3">
         <v>120</v>
@@ -7297,8 +7396,8 @@
       <c r="L122" s="3">
         <v>0</v>
       </c>
-      <c r="M122" s="8" t="b">
-        <v>0</v>
+      <c r="M122" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N122" s="3">
         <v>121</v>
@@ -7336,8 +7435,8 @@
       <c r="L123" s="3">
         <v>0</v>
       </c>
-      <c r="M123" s="8" t="b">
-        <v>0</v>
+      <c r="M123" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="N123" s="3">
         <v>122</v>
@@ -7378,8 +7477,8 @@
       <c r="L124" s="3">
         <v>0</v>
       </c>
-      <c r="M124" s="8" t="b">
-        <v>1</v>
+      <c r="M124" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N124" s="3">
         <v>123</v>
@@ -7420,8 +7519,8 @@
       <c r="L125" s="3">
         <v>0</v>
       </c>
-      <c r="M125" s="8" t="b">
-        <v>1</v>
+      <c r="M125" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N125" s="3">
         <v>124</v>
@@ -7462,8 +7561,8 @@
       <c r="L126" s="3">
         <v>0</v>
       </c>
-      <c r="M126" s="8" t="b">
-        <v>1</v>
+      <c r="M126" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="N126" s="3">
         <v>125</v>
@@ -7481,13 +7580,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C94FEBB1-315A-4609-9BCC-2B9E16A284E8}">
-          <x14:formula1>
-            <xm:f>Lookups!$M$3:$M$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>M2:M126</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{52DB5617-9AC6-42B3-A0A1-82418CF13405}">
           <x14:formula1>
             <xm:f>Lookups!$K$3:$K$9</xm:f>
@@ -7532,7 +7625,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9010,13 +9103,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A29F23-3414-4C7A-B10C-DD605B945639}">
-  <dimension ref="A1:G71"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9072,7 +9165,7 @@
         <v>211</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>66</v>
+        <v>249</v>
       </c>
       <c r="G2" s="3">
         <v>1</v>
@@ -9096,7 +9189,7 @@
         <v>213</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>66</v>
+        <v>250</v>
       </c>
       <c r="G3" s="3">
         <v>2</v>
@@ -9120,7 +9213,7 @@
         <v>214</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>66</v>
+        <v>251</v>
       </c>
       <c r="G4" s="3">
         <v>3</v>
@@ -9144,7 +9237,7 @@
         <v>216</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>66</v>
+        <v>252</v>
       </c>
       <c r="G5" s="3">
         <v>4</v>
@@ -9152,7 +9245,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="8">
         <v>3</v>
@@ -9161,22 +9254,22 @@
         <f>IF((B6=""),"",VLOOKUP(B6,Outcomes!$A$2:$D$101,4,FALSE))</f>
         <v>Proponent withdraws Submission from the Exemption Request process</v>
       </c>
-      <c r="D6" t="s">
-        <v>217</v>
+      <c r="D6" s="29" t="s">
+        <v>219</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>66</v>
+        <v>253</v>
       </c>
       <c r="G6" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="8">
         <v>3</v>
@@ -9186,93 +9279,93 @@
         <v>Proponent withdraws Submission from the Exemption Request process</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>66</v>
+        <v>254</v>
       </c>
       <c r="G7" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C8" s="6" t="str">
         <f>IF((B8=""),"",VLOOKUP(B8,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Proponent withdraws Submission from the Exemption Request process</v>
+        <v>Starts the "clock" for EAC Assessment</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>221</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>224</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>66</v>
+        <v>255</v>
       </c>
       <c r="G8" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C9" s="6" t="str">
         <f>IF((B9=""),"",VLOOKUP(B9,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Starts the "clock" for EAC Assessment</v>
+        <v>Dispute Resolution is started</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>66</v>
+        <v>256</v>
       </c>
       <c r="G9" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C10" s="6" t="str">
         <f>IF((B10=""),"",VLOOKUP(B10,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Dispute Resolution is started</v>
+        <v>Exemption Request is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>66</v>
+        <v>252</v>
       </c>
       <c r="G10" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B11" s="8">
         <v>6</v>
@@ -9282,21 +9375,21 @@
         <v>Exemption Request is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>216</v>
+        <v>227</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>66</v>
+        <v>257</v>
       </c>
       <c r="G11" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B12" s="8">
         <v>6</v>
@@ -9305,70 +9398,70 @@
         <f>IF((B12=""),"",VLOOKUP(B12,Outcomes!$A$2:$D$101,4,FALSE))</f>
         <v>Exemption Request is Terminated under s.39(d) of Act</v>
       </c>
-      <c r="D12" t="s">
-        <v>217</v>
+      <c r="D12" s="29" t="s">
+        <v>221</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>66</v>
+        <v>254</v>
       </c>
       <c r="G12" s="3">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13" s="8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C13" s="6" t="str">
         <f>IF((B13=""),"",VLOOKUP(B13,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Exemption Request is Terminated under s.39(d) of Act</v>
+        <v>Proponent withdraws Submission from the Exemption Request process</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E13" s="29" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>66</v>
+        <v>252</v>
       </c>
       <c r="G13" s="3">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B14" s="8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C14" s="6" t="str">
         <f>IF((B14=""),"",VLOOKUP(B14,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Exemption Request is Terminated under s.39(d) of Act</v>
+        <v>Proponent withdraws Submission from the Exemption Request process</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>66</v>
+        <v>253</v>
       </c>
       <c r="G14" s="3">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B15" s="8">
         <v>7</v>
@@ -9378,220 +9471,220 @@
         <v>Proponent withdraws Submission from the Exemption Request process</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="E15" s="29" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>66</v>
+        <v>254</v>
       </c>
       <c r="G15" s="3">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B16" s="8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C16" s="6" t="str">
         <f>IF((B16=""),"",VLOOKUP(B16,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Proponent withdraws Submission from the Exemption Request process</v>
-      </c>
-      <c r="D16" t="s">
-        <v>217</v>
-      </c>
-      <c r="E16" s="29" t="s">
-        <v>218</v>
+        <v>End of Early Engagement PHASE, start of DPD Development (Proponent Time) PHASE</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>228</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>66</v>
+        <v>258</v>
       </c>
       <c r="G16" s="3">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B17" s="8">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C17" s="6" t="str">
         <f>IF((B17=""),"",VLOOKUP(B17,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Proponent withdraws Submission from the Exemption Request process</v>
-      </c>
-      <c r="D17" s="29" t="s">
-        <v>219</v>
-      </c>
-      <c r="E17" s="29" t="s">
-        <v>220</v>
+        <v>Draft Detailed Project Description Initial Review is POSITIVE</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>229</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>66</v>
+        <v>259</v>
       </c>
       <c r="G17" s="3">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B18" s="8">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C18" s="6" t="str">
         <f>IF((B18=""),"",VLOOKUP(B18,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Proponent withdraws Submission from the Exemption Request process</v>
-      </c>
-      <c r="D18" s="29" t="s">
-        <v>221</v>
-      </c>
-      <c r="E18" s="29" t="s">
-        <v>222</v>
+        <v>Draft Detailed Project Description Initial Review is NEGATIVE</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>230</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>66</v>
+        <v>260</v>
       </c>
       <c r="G18" s="3">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B19" s="8">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C19" s="6" t="str">
         <f>IF((B19=""),"",VLOOKUP(B19,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>End of Early Engagement PHASE, start of DPD Development (Proponent Time) PHASE</v>
+        <v>Draft Detailed Project Description Initial Review is NEGATIVE</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>66</v>
+        <v>261</v>
       </c>
       <c r="G19" s="3">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B20" s="8">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C20" s="6" t="str">
         <f>IF((B20=""),"",VLOOKUP(B20,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Draft Detailed Project Description Initial Review is POSITIVE</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>229</v>
+        <v>Dispute Resolution is started</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="E20" s="29" t="s">
+        <v>226</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>66</v>
+        <v>256</v>
       </c>
       <c r="G20" s="3">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B21" s="8">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C21" s="6" t="str">
         <f>IF((B21=""),"",VLOOKUP(B21,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Draft Detailed Project Description Initial Review is NEGATIVE</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>230</v>
+        <v>Exemption Request is Terminated under s.39(d) of Act</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>215</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>216</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>66</v>
+        <v>252</v>
       </c>
       <c r="G21" s="3">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B22" s="8">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C22" s="6" t="str">
         <f>IF((B22=""),"",VLOOKUP(B22,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Draft Detailed Project Description Initial Review is NEGATIVE</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>231</v>
+        <v>Exemption Request is Terminated under s.39(d) of Act</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>219</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>227</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>66</v>
+        <v>257</v>
       </c>
       <c r="G22" s="3">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B23" s="8">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C23" s="6" t="str">
         <f>IF((B23=""),"",VLOOKUP(B23,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Dispute Resolution is started</v>
+        <v>Exemption Request is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E23" s="29" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>66</v>
+        <v>254</v>
       </c>
       <c r="G23" s="3">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B24" s="8">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C24" s="6" t="str">
         <f>IF((B24=""),"",VLOOKUP(B24,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Exemption Request is Terminated under s.39(d) of Act</v>
+        <v>Proponent withdraws Submission from the Exemption Request process</v>
       </c>
       <c r="D24" s="29" t="s">
         <v>215</v>
@@ -9600,354 +9693,354 @@
         <v>216</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>66</v>
+        <v>252</v>
       </c>
       <c r="G24" s="3">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B25" s="8">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C25" s="6" t="str">
         <f>IF((B25=""),"",VLOOKUP(B25,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Exemption Request is Terminated under s.39(d) of Act</v>
-      </c>
-      <c r="D25" t="s">
-        <v>217</v>
+        <v>Proponent withdraws Submission from the Exemption Request process</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>219</v>
       </c>
       <c r="E25" s="29" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>66</v>
+        <v>253</v>
       </c>
       <c r="G25" s="3">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B26" s="8">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C26" s="6" t="str">
         <f>IF((B26=""),"",VLOOKUP(B26,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Exemption Request is Terminated under s.39(d) of Act</v>
+        <v>Proponent withdraws Submission from the Exemption Request process</v>
       </c>
       <c r="D26" s="29" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="E26" s="29" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>66</v>
+        <v>254</v>
       </c>
       <c r="G26" s="3">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B27" s="8">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C27" s="6" t="str">
         <f>IF((B27=""),"",VLOOKUP(B27,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Exemption Request is Terminated under s.39(d) of Act</v>
-      </c>
-      <c r="D27" s="29" t="s">
-        <v>221</v>
+        <v>Proponent must submit a Revised DPD</v>
+      </c>
+      <c r="D27" t="s">
+        <v>217</v>
       </c>
       <c r="E27" s="29" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>66</v>
+        <v>252</v>
       </c>
       <c r="G27" s="3">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B28" s="8">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C28" s="6" t="str">
         <f>IF((B28=""),"",VLOOKUP(B28,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Proponent withdraws Submission from the Exemption Request process</v>
-      </c>
-      <c r="D28" s="29" t="s">
-        <v>215</v>
-      </c>
-      <c r="E28" s="29" t="s">
-        <v>216</v>
+        <v>Proponent must submit a Revised DPD</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>237</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>66</v>
+        <v>263</v>
       </c>
       <c r="G28" s="3">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B29" s="8">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C29" s="6" t="str">
         <f>IF((B29=""),"",VLOOKUP(B29,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Proponent withdraws Submission from the Exemption Request process</v>
-      </c>
-      <c r="D29" t="s">
-        <v>217</v>
-      </c>
-      <c r="E29" s="29" t="s">
-        <v>218</v>
+        <v>Proponent must submit a Revised DPD</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>233</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>66</v>
+        <v>264</v>
       </c>
       <c r="G29" s="3">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B30" s="8">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C30" s="6" t="str">
         <f>IF((B30=""),"",VLOOKUP(B30,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Proponent withdraws Submission from the Exemption Request process</v>
-      </c>
-      <c r="D30" s="29" t="s">
-        <v>219</v>
-      </c>
-      <c r="E30" s="29" t="s">
-        <v>220</v>
+        <v>Proponent must submit a Revised DPD</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>234</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>66</v>
+        <v>265</v>
       </c>
       <c r="G30" s="3">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B31" s="8">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C31" s="6" t="str">
         <f>IF((B31=""),"",VLOOKUP(B31,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Proponent withdraws Submission from the Exemption Request process</v>
-      </c>
-      <c r="D31" s="29" t="s">
-        <v>221</v>
-      </c>
-      <c r="E31" s="29" t="s">
-        <v>222</v>
+        <v>Proponent must submit a Revised DPD</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>235</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>66</v>
+        <v>266</v>
       </c>
       <c r="G31" s="3">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B32" s="8">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C32" s="6" t="str">
         <f>IF((B32=""),"",VLOOKUP(B32,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Proponent must submit a Revised DPD</v>
-      </c>
-      <c r="D32" t="s">
-        <v>217</v>
+        <v>Dispute Resolution is started</v>
+      </c>
+      <c r="D32" s="29" t="s">
+        <v>225</v>
       </c>
       <c r="E32" s="29" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>66</v>
+        <v>256</v>
       </c>
       <c r="G32" s="3">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B33" s="8">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C33" s="6" t="str">
         <f>IF((B33=""),"",VLOOKUP(B33,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Proponent must submit a Revised DPD</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>237</v>
+        <v>Exemption Request is Terminated under s.39(d) of Act</v>
+      </c>
+      <c r="D33" s="29" t="s">
+        <v>215</v>
+      </c>
+      <c r="E33" s="29" t="s">
+        <v>216</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>66</v>
+        <v>252</v>
       </c>
       <c r="G33" s="3">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B34" s="8">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C34" s="6" t="str">
         <f>IF((B34=""),"",VLOOKUP(B34,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Proponent must submit a Revised DPD</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>233</v>
+        <v>Exemption Request is Terminated under s.39(d) of Act</v>
+      </c>
+      <c r="D34" s="29" t="s">
+        <v>219</v>
+      </c>
+      <c r="E34" s="29" t="s">
+        <v>227</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>66</v>
+        <v>257</v>
       </c>
       <c r="G34" s="3">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B35" s="8">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C35" s="6" t="str">
         <f>IF((B35=""),"",VLOOKUP(B35,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Proponent must submit a Revised DPD</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>234</v>
+        <v>Exemption Request is Terminated under s.39(d) of Act</v>
+      </c>
+      <c r="D35" s="29" t="s">
+        <v>221</v>
+      </c>
+      <c r="E35" s="29" t="s">
+        <v>222</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>66</v>
+        <v>254</v>
       </c>
       <c r="G35" s="3">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B36" s="8">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C36" s="6" t="str">
         <f>IF((B36=""),"",VLOOKUP(B36,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Proponent must submit a Revised DPD</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>235</v>
+        <v>Proponent withdraws Submission from the Exemption Request process</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>215</v>
+      </c>
+      <c r="E36" s="29" t="s">
+        <v>216</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>66</v>
+        <v>252</v>
       </c>
       <c r="G36" s="3">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B37" s="8">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C37" s="6" t="str">
         <f>IF((B37=""),"",VLOOKUP(B37,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Project is Referred to Minister for Exemption</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>239</v>
+        <v>Proponent withdraws Submission from the Exemption Request process</v>
+      </c>
+      <c r="D37" s="29" t="s">
+        <v>219</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>220</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>66</v>
+        <v>253</v>
       </c>
       <c r="G37" s="3">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B38" s="8">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C38" s="6" t="str">
         <f>IF((B38=""),"",VLOOKUP(B38,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Dispute Resolution is started</v>
+        <v>Proponent withdraws Submission from the Exemption Request process</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>66</v>
+        <v>254</v>
       </c>
       <c r="G38" s="3">
-        <v>37</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B39" s="8">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C39" s="6" t="str">
         <f>IF((B39=""),"",VLOOKUP(B39,Outcomes!$A$2:$D$101,4,FALSE))</f>
@@ -9960,166 +10053,166 @@
         <v>216</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>66</v>
+        <v>252</v>
       </c>
       <c r="G39" s="3">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B40" s="8">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C40" s="6" t="str">
         <f>IF((B40=""),"",VLOOKUP(B40,Outcomes!$A$2:$D$101,4,FALSE))</f>
         <v>Exemption Request is Terminated under s.39(d) of Act</v>
       </c>
-      <c r="D40" t="s">
-        <v>217</v>
+      <c r="D40" s="29" t="s">
+        <v>219</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>66</v>
+        <v>257</v>
       </c>
       <c r="G40" s="3">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B41" s="8">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C41" s="6" t="str">
         <f>IF((B41=""),"",VLOOKUP(B41,Outcomes!$A$2:$D$101,4,FALSE))</f>
         <v>Exemption Request is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D41" s="29" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="E41" s="29" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>66</v>
+        <v>254</v>
       </c>
       <c r="G41" s="3">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B42" s="8">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C42" s="6" t="str">
         <f>IF((B42=""),"",VLOOKUP(B42,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Exemption Request is Terminated under s.39(d) of Act</v>
+        <v>Proponent withdraws Submission from the Exemption Request process</v>
       </c>
       <c r="D42" s="29" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="E42" s="29" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>66</v>
+        <v>252</v>
       </c>
       <c r="G42" s="3">
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B43" s="8">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C43" s="6" t="str">
         <f>IF((B43=""),"",VLOOKUP(B43,Outcomes!$A$2:$D$101,4,FALSE))</f>
         <v>Proponent withdraws Submission from the Exemption Request process</v>
       </c>
       <c r="D43" s="29" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="E43" s="29" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>66</v>
+        <v>253</v>
       </c>
       <c r="G43" s="3">
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B44" s="8">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C44" s="6" t="str">
         <f>IF((B44=""),"",VLOOKUP(B44,Outcomes!$A$2:$D$101,4,FALSE))</f>
         <v>Proponent withdraws Submission from the Exemption Request process</v>
       </c>
-      <c r="D44" t="s">
-        <v>217</v>
+      <c r="D44" s="29" t="s">
+        <v>221</v>
       </c>
       <c r="E44" s="29" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>66</v>
+        <v>254</v>
       </c>
       <c r="G44" s="3">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B45" s="8">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C45" s="6" t="str">
         <f>IF((B45=""),"",VLOOKUP(B45,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Proponent withdraws Submission from the Exemption Request process</v>
+        <v>Project is Exempt from Requiring an EAC</v>
       </c>
       <c r="D45" s="29" t="s">
         <v>219</v>
       </c>
       <c r="E45" s="29" t="s">
-        <v>220</v>
+        <v>267</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>66</v>
+        <v>268</v>
       </c>
       <c r="G45" s="3">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B46" s="8">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C46" s="6" t="str">
         <f>IF((B46=""),"",VLOOKUP(B46,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Proponent withdraws Submission from the Exemption Request process</v>
+        <v>Project is Exempt from Requiring an EAC</v>
       </c>
       <c r="D46" s="29" t="s">
         <v>221</v>
@@ -10128,162 +10221,162 @@
         <v>222</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>66</v>
+        <v>254</v>
       </c>
       <c r="G46" s="3">
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="B47" s="8">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C47" s="6" t="str">
         <f>IF((B47=""),"",VLOOKUP(B47,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Exemption Request is Terminated under s.39(d) of Act</v>
-      </c>
-      <c r="D47" s="29" t="s">
-        <v>215</v>
-      </c>
-      <c r="E47" s="29" t="s">
-        <v>216</v>
+        <v>Refer the Project to the CEAO for Further Decision</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>242</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>66</v>
+        <v>269</v>
       </c>
       <c r="G47" s="3">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="B48" s="8">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C48" s="6" t="str">
         <f>IF((B48=""),"",VLOOKUP(B48,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Exemption Request is Terminated under s.39(d) of Act</v>
-      </c>
-      <c r="D48" t="s">
-        <v>217</v>
-      </c>
-      <c r="E48" s="29" t="s">
-        <v>218</v>
+        <v>Refer the Project to the CEAO for Further Decision</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>243</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>66</v>
+        <v>270</v>
       </c>
       <c r="G48" s="3">
-        <v>47</v>
+        <v>57</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="B49" s="8">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C49" s="6" t="str">
         <f>IF((B49=""),"",VLOOKUP(B49,Outcomes!$A$2:$D$101,4,FALSE))</f>
         <v>Exemption Request is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D49" s="29" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E49" s="29" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>66</v>
+        <v>252</v>
       </c>
       <c r="G49" s="3">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B50" s="8">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C50" s="6" t="str">
         <f>IF((B50=""),"",VLOOKUP(B50,Outcomes!$A$2:$D$101,4,FALSE))</f>
         <v>Exemption Request is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D50" s="29" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E50" s="29" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>66</v>
+        <v>257</v>
       </c>
       <c r="G50" s="3">
-        <v>49</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="B51" s="8">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C51" s="6" t="str">
         <f>IF((B51=""),"",VLOOKUP(B51,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Proponent withdraws Submission from the Exemption Request process</v>
+        <v>Exemption Request is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D51" s="29" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="E51" s="29" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>66</v>
+        <v>254</v>
       </c>
       <c r="G51" s="3">
-        <v>50</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="B52" s="8">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C52" s="6" t="str">
         <f>IF((B52=""),"",VLOOKUP(B52,Outcomes!$A$2:$D$101,4,FALSE))</f>
         <v>Proponent withdraws Submission from the Exemption Request process</v>
       </c>
-      <c r="D52" t="s">
-        <v>217</v>
+      <c r="D52" s="29" t="s">
+        <v>215</v>
       </c>
       <c r="E52" s="29" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>66</v>
+        <v>252</v>
       </c>
       <c r="G52" s="3">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B53" s="8">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C53" s="6" t="str">
         <f>IF((B53=""),"",VLOOKUP(B53,Outcomes!$A$2:$D$101,4,FALSE))</f>
@@ -10296,18 +10389,18 @@
         <v>220</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>66</v>
+        <v>253</v>
       </c>
       <c r="G53" s="3">
-        <v>52</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="B54" s="8">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C54" s="6" t="str">
         <f>IF((B54=""),"",VLOOKUP(B54,Outcomes!$A$2:$D$101,4,FALSE))</f>
@@ -10320,417 +10413,129 @@
         <v>222</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>66</v>
+        <v>254</v>
       </c>
       <c r="G54" s="3">
-        <v>53</v>
+        <v>65</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="B55" s="8">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C55" s="6" t="str">
         <f>IF((B55=""),"",VLOOKUP(B55,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Project is Exempt from Requiring an EAC</v>
-      </c>
-      <c r="D55" s="29" t="s">
-        <v>219</v>
-      </c>
-      <c r="E55" s="29" t="s">
-        <v>241</v>
+        <v>Proponent must submit a Revised DPD</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>233</v>
       </c>
       <c r="F55" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="G55" s="3">
         <v>66</v>
-      </c>
-      <c r="G55" s="3">
-        <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="B56" s="8">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C56" s="6" t="str">
         <f>IF((B56=""),"",VLOOKUP(B56,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Project is Exempt from Requiring an EAC</v>
-      </c>
-      <c r="D56" s="29" t="s">
-        <v>221</v>
-      </c>
-      <c r="E56" s="29" t="s">
-        <v>222</v>
+        <v>Proponent must submit a Revised DPD</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>234</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>66</v>
+        <v>265</v>
       </c>
       <c r="G56" s="3">
-        <v>55</v>
+        <v>67</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="B57" s="8">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C57" s="6" t="str">
         <f>IF((B57=""),"",VLOOKUP(B57,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Refer the Project to the CEAO for Further Decision</v>
+        <v>Proponent must submit a Revised DPD</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>66</v>
+        <v>266</v>
       </c>
       <c r="G57" s="3">
-        <v>56</v>
+        <v>68</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="B58" s="8">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C58" s="6" t="str">
         <f>IF((B58=""),"",VLOOKUP(B58,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Refer the Project to the CEAO for Further Decision</v>
+        <v>Project moves to Process Planning</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>66</v>
       </c>
       <c r="G58" s="3">
-        <v>57</v>
+        <v>69</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="B59" s="8">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C59" s="6" t="str">
         <f>IF((B59=""),"",VLOOKUP(B59,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Exemption Request is Terminated under s.39(d) of Act</v>
-      </c>
-      <c r="D59" s="29" t="s">
-        <v>215</v>
-      </c>
-      <c r="E59" s="29" t="s">
-        <v>216</v>
+        <v>Project moves to Process Planning</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>244</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>66</v>
       </c>
       <c r="G59" s="3">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="3">
-        <v>59</v>
-      </c>
-      <c r="B60" s="8">
-        <v>23</v>
-      </c>
-      <c r="C60" s="6" t="str">
-        <f>IF((B60=""),"",VLOOKUP(B60,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Exemption Request is Terminated under s.39(d) of Act</v>
-      </c>
-      <c r="D60" t="s">
-        <v>217</v>
-      </c>
-      <c r="E60" s="29" t="s">
-        <v>218</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G60" s="3">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" s="3">
-        <v>60</v>
-      </c>
-      <c r="B61" s="8">
-        <v>23</v>
-      </c>
-      <c r="C61" s="6" t="str">
-        <f>IF((B61=""),"",VLOOKUP(B61,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Exemption Request is Terminated under s.39(d) of Act</v>
-      </c>
-      <c r="D61" s="29" t="s">
-        <v>219</v>
-      </c>
-      <c r="E61" s="29" t="s">
-        <v>227</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G61" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" s="3">
-        <v>61</v>
-      </c>
-      <c r="B62" s="8">
-        <v>23</v>
-      </c>
-      <c r="C62" s="6" t="str">
-        <f>IF((B62=""),"",VLOOKUP(B62,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Exemption Request is Terminated under s.39(d) of Act</v>
-      </c>
-      <c r="D62" s="29" t="s">
-        <v>221</v>
-      </c>
-      <c r="E62" s="29" t="s">
-        <v>222</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G62" s="3">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" s="3">
-        <v>62</v>
-      </c>
-      <c r="B63" s="8">
-        <v>24</v>
-      </c>
-      <c r="C63" s="6" t="str">
-        <f>IF((B63=""),"",VLOOKUP(B63,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Proponent withdraws Submission from the Exemption Request process</v>
-      </c>
-      <c r="D63" s="29" t="s">
-        <v>215</v>
-      </c>
-      <c r="E63" s="29" t="s">
-        <v>216</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G63" s="3">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A64" s="3">
-        <v>63</v>
-      </c>
-      <c r="B64" s="8">
-        <v>24</v>
-      </c>
-      <c r="C64" s="6" t="str">
-        <f>IF((B64=""),"",VLOOKUP(B64,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Proponent withdraws Submission from the Exemption Request process</v>
-      </c>
-      <c r="D64" t="s">
-        <v>217</v>
-      </c>
-      <c r="E64" s="29" t="s">
-        <v>218</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G64" s="3">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A65" s="3">
-        <v>64</v>
-      </c>
-      <c r="B65" s="8">
-        <v>24</v>
-      </c>
-      <c r="C65" s="6" t="str">
-        <f>IF((B65=""),"",VLOOKUP(B65,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Proponent withdraws Submission from the Exemption Request process</v>
-      </c>
-      <c r="D65" s="29" t="s">
-        <v>219</v>
-      </c>
-      <c r="E65" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G65" s="3">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A66" s="3">
-        <v>65</v>
-      </c>
-      <c r="B66" s="8">
-        <v>24</v>
-      </c>
-      <c r="C66" s="6" t="str">
-        <f>IF((B66=""),"",VLOOKUP(B66,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Proponent withdraws Submission from the Exemption Request process</v>
-      </c>
-      <c r="D66" s="29" t="s">
-        <v>221</v>
-      </c>
-      <c r="E66" s="29" t="s">
-        <v>222</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G66" s="3">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A67" s="3">
-        <v>66</v>
-      </c>
-      <c r="B67" s="8">
-        <v>25</v>
-      </c>
-      <c r="C67" s="6" t="str">
-        <f>IF((B67=""),"",VLOOKUP(B67,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Proponent must submit a Revised DPD</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G67" s="3">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A68" s="3">
-        <v>67</v>
-      </c>
-      <c r="B68" s="8">
-        <v>25</v>
-      </c>
-      <c r="C68" s="6" t="str">
-        <f>IF((B68=""),"",VLOOKUP(B68,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Proponent must submit a Revised DPD</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G68" s="3">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A69" s="3">
-        <v>68</v>
-      </c>
-      <c r="B69" s="8">
-        <v>25</v>
-      </c>
-      <c r="C69" s="6" t="str">
-        <f>IF((B69=""),"",VLOOKUP(B69,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Proponent must submit a Revised DPD</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="F69" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G69" s="3">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A70" s="3">
-        <v>69</v>
-      </c>
-      <c r="B70" s="8">
-        <v>26</v>
-      </c>
-      <c r="C70" s="6" t="str">
-        <f>IF((B70=""),"",VLOOKUP(B70,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Project moves to Process Planning</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G70" s="3">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" s="3">
-        <v>70</v>
-      </c>
-      <c r="B71" s="8">
-        <v>26</v>
-      </c>
-      <c r="C71" s="6" t="str">
-        <f>IF((B71=""),"",VLOOKUP(B71,Outcomes!$A$2:$D$101,4,FALSE))</f>
-        <v>Project moves to Process Planning</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="F71" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G71" s="3">
         <v>70</v>
       </c>
     </row>
@@ -10743,7 +10548,7 @@
           <x14:formula1>
             <xm:f>Outcomes!$A$2:$A$101</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B71</xm:sqref>
+          <xm:sqref>B2:B59</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -10752,6 +10557,57 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEDB645B-9832-43C9-93CA-B4DC05EC6BC0}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3">
+        <v>36</v>
+      </c>
+      <c r="B1" s="8">
+        <v>15</v>
+      </c>
+      <c r="C1" s="6" t="str">
+        <f>IF((B1=""),"",VLOOKUP(B1,Outcomes!$A$2:$D$101,4,FALSE))</f>
+        <v>Project is Referred to Minister for Exemption</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="3">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CD376E2D-0D02-46B5-8EB4-1C59799E70C5}">
+          <x14:formula1>
+            <xm:f>Outcomes!$A$2:$A$101</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE27281F-AEB4-48A9-B0E8-27AC02018115}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>

</xml_diff>

<commit_message>
Exemption_Request template file fixes
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/exemption_request/001_Exemption_Request.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/exemption_request/001_Exemption_Request.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\eao\beta\code\epictrack-api\src\api\templates\event_templates\exemption_request\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E25389-8E21-435D-BE5D-E40194146CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC74BE90-31EE-4460-8EE8-9BB845619487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="274">
   <si>
     <t>No</t>
   </si>
@@ -940,9 +940,6 @@
     <t>Last Day of Exemption Request Readiness Decision (Date Capture Milestone)</t>
   </si>
   <si>
-    <t>Set workState to COMPLETE</t>
-  </si>
-  <si>
     <t>Set "Further Readiness Decision" PHASE to ACTIVE (show it)</t>
   </si>
   <si>
@@ -967,9 +964,6 @@
     <t>{"phase_name":"Exemption Early Engagement","work_type_id": 5, "ea_act_id": 3, "event_name": "Approval of IPD/EP Submission", "start_at": 1 }</t>
   </si>
   <si>
-    <t>{"phase_name":"Exemption Request Intake","work_type_id": 5, "ea_act_id": 3, "event_name": "Submission of "Draft" Initial Project Description &amp; Engagement Plan", "start_at": 21 }</t>
-  </si>
-  <si>
     <t>{"phase_name":"Exemption Request Intake","work_type_id": 5, "ea_act_id": 3, "event_name": "\"Draft\" Initial Project Description &amp; Engagement Plan Initial Review", "start_at": 28 }</t>
   </si>
   <si>
@@ -1028,6 +1022,21 @@
   </si>
   <si>
     <t>{"phase_name":"Further Readiness Decision","work_type_id": 5, "ea_act_id": 3, "event_name": "Readiness Decision Report referred to CEAO for Further Decision", "start_at": 1}</t>
+  </si>
+  <si>
+    <t>{"work_type": 6}</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Exemption DPD Development (Proponent Time)","work_type_id": 5, "ea_act_id": 3, "new_name": "Revised Exemption DPD Development (Proponent Time)", "legislated": false }</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Exemption Readiness Decision","work_type_id": 5, "ea_act_id": 3, "new_name": "Revised Exemption Readiness Decision", "legislated": false }</t>
+  </si>
+  <si>
+    <t>Exemption Order</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Exemption Request Intake","work_type_id": 5, "ea_act_id": 3, "event_name": "Submission of \"Draft\" Initial Project Description &amp; Engagement Plan", "start_at": 21 }</t>
   </si>
 </sst>
 </file>
@@ -1687,7 +1696,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1724,7 +1733,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -1738,7 +1747,7 @@
         <v>108</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>105</v>
+        <v>272</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>20</v>
@@ -1753,7 +1762,7 @@
         <v>65</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I2" s="3">
         <v>1</v>
@@ -1767,7 +1776,7 @@
         <v>109</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>105</v>
+        <v>272</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>20</v>
@@ -1782,7 +1791,7 @@
         <v>65</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I3" s="3">
         <v>2</v>
@@ -1796,7 +1805,7 @@
         <v>110</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>105</v>
+        <v>272</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>20</v>
@@ -1811,7 +1820,7 @@
         <v>65</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I4" s="3">
         <v>3</v>
@@ -1825,7 +1834,7 @@
         <v>111</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>105</v>
+        <v>272</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>20</v>
@@ -1840,7 +1849,7 @@
         <v>65</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I5" s="3">
         <v>4</v>
@@ -1854,7 +1863,7 @@
         <v>112</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>105</v>
+        <v>272</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>20</v>
@@ -1869,7 +1878,7 @@
         <v>65</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I6" s="3">
         <v>5</v>
@@ -1883,7 +1892,7 @@
         <v>113</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>105</v>
+        <v>272</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>20</v>
@@ -1898,7 +1907,7 @@
         <v>65</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="I7" s="3">
         <v>6</v>
@@ -2385,7 +2394,7 @@
   <dimension ref="A1:N126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="E65" sqref="E65"/>
@@ -2441,7 +2450,7 @@
         <v>4</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>7</v>
@@ -2480,7 +2489,7 @@
         <v>0</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N2" s="3">
         <v>1</v>
@@ -2519,7 +2528,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N3" s="3">
         <v>2</v>
@@ -2558,7 +2567,7 @@
         <v>0</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N4" s="3">
         <v>3</v>
@@ -2600,7 +2609,7 @@
         <v>0</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N5" s="3">
         <v>4</v>
@@ -2639,7 +2648,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N6" s="3">
         <v>5</v>
@@ -2678,7 +2687,7 @@
         <v>0</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N7" s="3">
         <v>6</v>
@@ -2720,7 +2729,7 @@
         <v>0</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N8" s="3">
         <v>7</v>
@@ -2762,7 +2771,7 @@
         <v>0</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N9" s="3">
         <v>8</v>
@@ -2801,7 +2810,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N10" s="3">
         <v>9</v>
@@ -2843,7 +2852,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N11" s="3">
         <v>10</v>
@@ -2882,7 +2891,7 @@
         <v>0</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N12" s="3">
         <v>11</v>
@@ -2921,7 +2930,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N13" s="3">
         <v>12</v>
@@ -2963,7 +2972,7 @@
         <v>0</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N14" s="3">
         <v>13</v>
@@ -3005,7 +3014,7 @@
         <v>0</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N15" s="3">
         <v>14</v>
@@ -3047,7 +3056,7 @@
         <v>0</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N16" s="3">
         <v>15</v>
@@ -3086,7 +3095,7 @@
         <v>0</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N17" s="3">
         <v>16</v>
@@ -3125,7 +3134,7 @@
         <v>30</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N18" s="3">
         <v>17</v>
@@ -3167,7 +3176,7 @@
         <v>0</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N19" s="3">
         <v>18</v>
@@ -3209,7 +3218,7 @@
         <v>0</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N20" s="3">
         <v>19</v>
@@ -3251,7 +3260,7 @@
         <v>0</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N21" s="3">
         <v>20</v>
@@ -3293,7 +3302,7 @@
         <v>0</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N22" s="3">
         <v>21</v>
@@ -3332,7 +3341,7 @@
         <v>0</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N23" s="3">
         <v>22</v>
@@ -3374,7 +3383,7 @@
         <v>0</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N24" s="3">
         <v>23</v>
@@ -3413,7 +3422,7 @@
         <v>0</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N25" s="3">
         <v>24</v>
@@ -3455,7 +3464,7 @@
         <v>0</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N26" s="3">
         <v>25</v>
@@ -3494,7 +3503,7 @@
         <v>0</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N27" s="3">
         <v>26</v>
@@ -3533,7 +3542,7 @@
         <v>0</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N28" s="3">
         <v>27</v>
@@ -3575,7 +3584,7 @@
         <v>0</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N29" s="3">
         <v>28</v>
@@ -3614,7 +3623,7 @@
         <v>0</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N30" s="3">
         <v>29</v>
@@ -3653,7 +3662,7 @@
         <v>0</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N31" s="3">
         <v>30</v>
@@ -3695,7 +3704,7 @@
         <v>0</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N32" s="3">
         <v>31</v>
@@ -3737,7 +3746,7 @@
         <v>0</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N33" s="3">
         <v>32</v>
@@ -3779,7 +3788,7 @@
         <v>0</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N34" s="3">
         <v>33</v>
@@ -3821,7 +3830,7 @@
         <v>0</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N35" s="3">
         <v>34</v>
@@ -3860,7 +3869,7 @@
         <v>30</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N36" s="3">
         <v>35</v>
@@ -3902,7 +3911,7 @@
         <v>0</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N37" s="3">
         <v>36</v>
@@ -3944,7 +3953,7 @@
         <v>0</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N38" s="3">
         <v>37</v>
@@ -3986,7 +3995,7 @@
         <v>0</v>
       </c>
       <c r="M39" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N39" s="3">
         <v>38</v>
@@ -4028,7 +4037,7 @@
         <v>0</v>
       </c>
       <c r="M40" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N40" s="3">
         <v>39</v>
@@ -4067,7 +4076,7 @@
         <v>0</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N41" s="3">
         <v>40</v>
@@ -4106,7 +4115,7 @@
         <v>0</v>
       </c>
       <c r="M42" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N42" s="3">
         <v>41</v>
@@ -4145,7 +4154,7 @@
         <v>0</v>
       </c>
       <c r="M43" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N43" s="3">
         <v>42</v>
@@ -4187,7 +4196,7 @@
         <v>0</v>
       </c>
       <c r="M44" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N44" s="3">
         <v>43</v>
@@ -4229,7 +4238,7 @@
         <v>0</v>
       </c>
       <c r="M45" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N45" s="3">
         <v>44</v>
@@ -4268,7 +4277,7 @@
         <v>0</v>
       </c>
       <c r="M46" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N46" s="3">
         <v>45</v>
@@ -4310,7 +4319,7 @@
         <v>0</v>
       </c>
       <c r="M47" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N47" s="3">
         <v>46</v>
@@ -4352,7 +4361,7 @@
         <v>0</v>
       </c>
       <c r="M48" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N48" s="3">
         <v>47</v>
@@ -4391,7 +4400,7 @@
         <v>0</v>
       </c>
       <c r="M49" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N49" s="3">
         <v>48</v>
@@ -4433,7 +4442,7 @@
         <v>0</v>
       </c>
       <c r="M50" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N50" s="3">
         <v>49</v>
@@ -4475,7 +4484,7 @@
         <v>0</v>
       </c>
       <c r="M51" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N51" s="3">
         <v>50</v>
@@ -4514,7 +4523,7 @@
         <v>0</v>
       </c>
       <c r="M52" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N52" s="3">
         <v>51</v>
@@ -4556,7 +4565,7 @@
         <v>0</v>
       </c>
       <c r="M53" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N53" s="3">
         <v>52</v>
@@ -4598,7 +4607,7 @@
         <v>0</v>
       </c>
       <c r="M54" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N54" s="3">
         <v>53</v>
@@ -4640,7 +4649,7 @@
         <v>0</v>
       </c>
       <c r="M55" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N55" s="3">
         <v>54</v>
@@ -4682,7 +4691,7 @@
         <v>0</v>
       </c>
       <c r="M56" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N56" s="3">
         <v>55</v>
@@ -4724,7 +4733,7 @@
         <v>0</v>
       </c>
       <c r="M57" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N57" s="3">
         <v>56</v>
@@ -4766,7 +4775,7 @@
         <v>0</v>
       </c>
       <c r="M58" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N58" s="3">
         <v>57</v>
@@ -4808,7 +4817,7 @@
         <v>0</v>
       </c>
       <c r="M59" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N59" s="3">
         <v>58</v>
@@ -4850,7 +4859,7 @@
         <v>0</v>
       </c>
       <c r="M60" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N60" s="3">
         <v>59</v>
@@ -4889,7 +4898,7 @@
         <v>0</v>
       </c>
       <c r="M61" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N61" s="3">
         <v>60</v>
@@ -4931,7 +4940,7 @@
         <v>0</v>
       </c>
       <c r="M62" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N62" s="3">
         <v>61</v>
@@ -4973,7 +4982,7 @@
         <v>0</v>
       </c>
       <c r="M63" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N63" s="3">
         <v>62</v>
@@ -5015,7 +5024,7 @@
         <v>0</v>
       </c>
       <c r="M64" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N64" s="3">
         <v>63</v>
@@ -5054,7 +5063,7 @@
         <v>0</v>
       </c>
       <c r="M65" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N65" s="3">
         <v>64</v>
@@ -5093,7 +5102,7 @@
         <v>0</v>
       </c>
       <c r="M66" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N66" s="3">
         <v>65</v>
@@ -5132,7 +5141,7 @@
         <v>0</v>
       </c>
       <c r="M67" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N67" s="3">
         <v>66</v>
@@ -5174,7 +5183,7 @@
         <v>0</v>
       </c>
       <c r="M68" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N68" s="3">
         <v>67</v>
@@ -5216,7 +5225,7 @@
         <v>0</v>
       </c>
       <c r="M69" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N69" s="3">
         <v>68</v>
@@ -5255,7 +5264,7 @@
         <v>0</v>
       </c>
       <c r="M70" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N70" s="3">
         <v>69</v>
@@ -5297,7 +5306,7 @@
         <v>0</v>
       </c>
       <c r="M71" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N71" s="3">
         <v>70</v>
@@ -5339,7 +5348,7 @@
         <v>0</v>
       </c>
       <c r="M72" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N72" s="3">
         <v>71</v>
@@ -5381,7 +5390,7 @@
         <v>0</v>
       </c>
       <c r="M73" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N73" s="3">
         <v>72</v>
@@ -5423,7 +5432,7 @@
         <v>0</v>
       </c>
       <c r="M74" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N74" s="3">
         <v>73</v>
@@ -5465,7 +5474,7 @@
         <v>0</v>
       </c>
       <c r="M75" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N75" s="3">
         <v>74</v>
@@ -5507,7 +5516,7 @@
         <v>0</v>
       </c>
       <c r="M76" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N76" s="3">
         <v>75</v>
@@ -5549,7 +5558,7 @@
         <v>0</v>
       </c>
       <c r="M77" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N77" s="3">
         <v>76</v>
@@ -5591,7 +5600,7 @@
         <v>0</v>
       </c>
       <c r="M78" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N78" s="3">
         <v>77</v>
@@ -5633,7 +5642,7 @@
         <v>0</v>
       </c>
       <c r="M79" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N79" s="3">
         <v>78</v>
@@ -5672,7 +5681,7 @@
         <v>0</v>
       </c>
       <c r="M80" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N80" s="3">
         <v>79</v>
@@ -5711,7 +5720,7 @@
         <v>0</v>
       </c>
       <c r="M81" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N81" s="3">
         <v>80</v>
@@ -5750,7 +5759,7 @@
         <v>0</v>
       </c>
       <c r="M82" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N82" s="3">
         <v>81</v>
@@ -5792,7 +5801,7 @@
         <v>0</v>
       </c>
       <c r="M83" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N83" s="3">
         <v>82</v>
@@ -5834,7 +5843,7 @@
         <v>0</v>
       </c>
       <c r="M84" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N84" s="3">
         <v>83</v>
@@ -5873,7 +5882,7 @@
         <v>0</v>
       </c>
       <c r="M85" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N85" s="3">
         <v>84</v>
@@ -5912,7 +5921,7 @@
         <v>0</v>
       </c>
       <c r="M86" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N86" s="3">
         <v>85</v>
@@ -5954,7 +5963,7 @@
         <v>0</v>
       </c>
       <c r="M87" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N87" s="3">
         <v>86</v>
@@ -5996,7 +6005,7 @@
         <v>0</v>
       </c>
       <c r="M88" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N88" s="3">
         <v>87</v>
@@ -6038,7 +6047,7 @@
         <v>0</v>
       </c>
       <c r="M89" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N89" s="3">
         <v>88</v>
@@ -6080,7 +6089,7 @@
         <v>0</v>
       </c>
       <c r="M90" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N90" s="3">
         <v>89</v>
@@ -6119,7 +6128,7 @@
         <v>0</v>
       </c>
       <c r="M91" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N91" s="3">
         <v>90</v>
@@ -6158,7 +6167,7 @@
         <v>0</v>
       </c>
       <c r="M92" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N92" s="3">
         <v>91</v>
@@ -6200,7 +6209,7 @@
         <v>0</v>
       </c>
       <c r="M93" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N93" s="3">
         <v>92</v>
@@ -6242,7 +6251,7 @@
         <v>0</v>
       </c>
       <c r="M94" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N94" s="3">
         <v>93</v>
@@ -6284,7 +6293,7 @@
         <v>0</v>
       </c>
       <c r="M95" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N95" s="3">
         <v>94</v>
@@ -6326,7 +6335,7 @@
         <v>0</v>
       </c>
       <c r="M96" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N96" s="3">
         <v>95</v>
@@ -6368,7 +6377,7 @@
         <v>0</v>
       </c>
       <c r="M97" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N97" s="3">
         <v>96</v>
@@ -6410,7 +6419,7 @@
         <v>0</v>
       </c>
       <c r="M98" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N98" s="3">
         <v>97</v>
@@ -6452,7 +6461,7 @@
         <v>0</v>
       </c>
       <c r="M99" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N99" s="3">
         <v>98</v>
@@ -6494,7 +6503,7 @@
         <v>0</v>
       </c>
       <c r="M100" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N100" s="3">
         <v>99</v>
@@ -6536,7 +6545,7 @@
         <v>0</v>
       </c>
       <c r="M101" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N101" s="3">
         <v>100</v>
@@ -6575,7 +6584,7 @@
         <v>0</v>
       </c>
       <c r="M102" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N102" s="3">
         <v>101</v>
@@ -6614,7 +6623,7 @@
         <v>0</v>
       </c>
       <c r="M103" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N103" s="3">
         <v>102</v>
@@ -6653,7 +6662,7 @@
         <v>0</v>
       </c>
       <c r="M104" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N104" s="3">
         <v>103</v>
@@ -6692,7 +6701,7 @@
         <v>0</v>
       </c>
       <c r="M105" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N105" s="3">
         <v>104</v>
@@ -6734,7 +6743,7 @@
         <v>0</v>
       </c>
       <c r="M106" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N106" s="3">
         <v>105</v>
@@ -6776,7 +6785,7 @@
         <v>0</v>
       </c>
       <c r="M107" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N107" s="3">
         <v>106</v>
@@ -6818,7 +6827,7 @@
         <v>0</v>
       </c>
       <c r="M108" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N108" s="3">
         <v>107</v>
@@ -6860,7 +6869,7 @@
         <v>0</v>
       </c>
       <c r="M109" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N109" s="3">
         <v>108</v>
@@ -6902,7 +6911,7 @@
         <v>0</v>
       </c>
       <c r="M110" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N110" s="3">
         <v>109</v>
@@ -6944,7 +6953,7 @@
         <v>0</v>
       </c>
       <c r="M111" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N111" s="3">
         <v>110</v>
@@ -6983,7 +6992,7 @@
         <v>0</v>
       </c>
       <c r="M112" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N112" s="3">
         <v>111</v>
@@ -7025,7 +7034,7 @@
         <v>0</v>
       </c>
       <c r="M113" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N113" s="3">
         <v>112</v>
@@ -7067,7 +7076,7 @@
         <v>0</v>
       </c>
       <c r="M114" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N114" s="3">
         <v>113</v>
@@ -7106,7 +7115,7 @@
         <v>0</v>
       </c>
       <c r="M115" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N115" s="3">
         <v>114</v>
@@ -7145,7 +7154,7 @@
         <v>0</v>
       </c>
       <c r="M116" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N116" s="3">
         <v>115</v>
@@ -7187,7 +7196,7 @@
         <v>0</v>
       </c>
       <c r="M117" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N117" s="3">
         <v>116</v>
@@ -7229,7 +7238,7 @@
         <v>0</v>
       </c>
       <c r="M118" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N118" s="3">
         <v>117</v>
@@ -7271,7 +7280,7 @@
         <v>0</v>
       </c>
       <c r="M119" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N119" s="3">
         <v>118</v>
@@ -7313,7 +7322,7 @@
         <v>0</v>
       </c>
       <c r="M120" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N120" s="3">
         <v>119</v>
@@ -7355,7 +7364,7 @@
         <v>0</v>
       </c>
       <c r="M121" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N121" s="3">
         <v>120</v>
@@ -7397,7 +7406,7 @@
         <v>0</v>
       </c>
       <c r="M122" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N122" s="3">
         <v>121</v>
@@ -7436,7 +7445,7 @@
         <v>0</v>
       </c>
       <c r="M123" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N123" s="3">
         <v>122</v>
@@ -7478,7 +7487,7 @@
         <v>0</v>
       </c>
       <c r="M124" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N124" s="3">
         <v>123</v>
@@ -7520,7 +7529,7 @@
         <v>0</v>
       </c>
       <c r="M125" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N125" s="3">
         <v>124</v>
@@ -7562,7 +7571,7 @@
         <v>0</v>
       </c>
       <c r="M126" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N126" s="3">
         <v>125</v>
@@ -9106,10 +9115,10 @@
   <dimension ref="A1:G59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E48" sqref="E48"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9165,7 +9174,7 @@
         <v>211</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G2" s="3">
         <v>1</v>
@@ -9189,7 +9198,7 @@
         <v>213</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>250</v>
+        <v>273</v>
       </c>
       <c r="G3" s="3">
         <v>2</v>
@@ -9213,7 +9222,7 @@
         <v>214</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G4" s="3">
         <v>3</v>
@@ -9237,7 +9246,7 @@
         <v>216</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G5" s="3">
         <v>4</v>
@@ -9261,7 +9270,7 @@
         <v>220</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G6" s="3">
         <v>6</v>
@@ -9285,7 +9294,7 @@
         <v>222</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G7" s="3">
         <v>7</v>
@@ -9309,7 +9318,7 @@
         <v>224</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="G8" s="3">
         <v>8</v>
@@ -9333,7 +9342,7 @@
         <v>226</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G9" s="3">
         <v>9</v>
@@ -9357,7 +9366,7 @@
         <v>216</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G10" s="3">
         <v>10</v>
@@ -9381,7 +9390,7 @@
         <v>227</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G11" s="3">
         <v>12</v>
@@ -9405,7 +9414,7 @@
         <v>222</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G12" s="3">
         <v>13</v>
@@ -9429,7 +9438,7 @@
         <v>216</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G13" s="3">
         <v>14</v>
@@ -9453,7 +9462,7 @@
         <v>220</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G14" s="3">
         <v>16</v>
@@ -9477,7 +9486,7 @@
         <v>222</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G15" s="3">
         <v>17</v>
@@ -9501,7 +9510,7 @@
         <v>228</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="G16" s="3">
         <v>18</v>
@@ -9525,7 +9534,7 @@
         <v>229</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G17" s="3">
         <v>19</v>
@@ -9549,7 +9558,7 @@
         <v>230</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G18" s="3">
         <v>20</v>
@@ -9573,7 +9582,7 @@
         <v>231</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G19" s="3">
         <v>21</v>
@@ -9597,7 +9606,7 @@
         <v>226</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G20" s="3">
         <v>22</v>
@@ -9621,7 +9630,7 @@
         <v>216</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G21" s="3">
         <v>23</v>
@@ -9645,7 +9654,7 @@
         <v>227</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G22" s="3">
         <v>25</v>
@@ -9669,7 +9678,7 @@
         <v>222</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G23" s="3">
         <v>26</v>
@@ -9693,7 +9702,7 @@
         <v>216</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G24" s="3">
         <v>27</v>
@@ -9717,7 +9726,7 @@
         <v>220</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G25" s="3">
         <v>29</v>
@@ -9741,7 +9750,7 @@
         <v>222</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G26" s="3">
         <v>30</v>
@@ -9765,7 +9774,7 @@
         <v>218</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G27" s="3">
         <v>31</v>
@@ -9789,7 +9798,7 @@
         <v>237</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G28" s="3">
         <v>32</v>
@@ -9813,7 +9822,7 @@
         <v>233</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G29" s="3">
         <v>33</v>
@@ -9837,7 +9846,7 @@
         <v>234</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G30" s="3">
         <v>34</v>
@@ -9861,7 +9870,7 @@
         <v>235</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G31" s="3">
         <v>35</v>
@@ -9885,7 +9894,7 @@
         <v>226</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G32" s="3">
         <v>37</v>
@@ -9909,7 +9918,7 @@
         <v>216</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G33" s="3">
         <v>38</v>
@@ -9933,7 +9942,7 @@
         <v>227</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G34" s="3">
         <v>40</v>
@@ -9957,7 +9966,7 @@
         <v>222</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G35" s="3">
         <v>41</v>
@@ -9981,7 +9990,7 @@
         <v>216</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G36" s="3">
         <v>42</v>
@@ -10005,7 +10014,7 @@
         <v>220</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G37" s="3">
         <v>44</v>
@@ -10029,7 +10038,7 @@
         <v>222</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G38" s="3">
         <v>45</v>
@@ -10053,7 +10062,7 @@
         <v>216</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G39" s="3">
         <v>46</v>
@@ -10077,7 +10086,7 @@
         <v>227</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G40" s="3">
         <v>48</v>
@@ -10101,7 +10110,7 @@
         <v>222</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G41" s="3">
         <v>49</v>
@@ -10125,7 +10134,7 @@
         <v>216</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G42" s="3">
         <v>50</v>
@@ -10149,7 +10158,7 @@
         <v>220</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G43" s="3">
         <v>52</v>
@@ -10173,7 +10182,7 @@
         <v>222</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G44" s="3">
         <v>53</v>
@@ -10194,10 +10203,10 @@
         <v>219</v>
       </c>
       <c r="E45" s="29" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G45" s="3">
         <v>54</v>
@@ -10221,7 +10230,7 @@
         <v>222</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G46" s="3">
         <v>55</v>
@@ -10242,10 +10251,10 @@
         <v>232</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G47" s="3">
         <v>56</v>
@@ -10266,10 +10275,10 @@
         <v>210</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G48" s="3">
         <v>57</v>
@@ -10293,7 +10302,7 @@
         <v>216</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G49" s="3">
         <v>58</v>
@@ -10317,7 +10326,7 @@
         <v>227</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G50" s="3">
         <v>60</v>
@@ -10341,7 +10350,7 @@
         <v>222</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G51" s="3">
         <v>61</v>
@@ -10365,7 +10374,7 @@
         <v>216</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G52" s="3">
         <v>62</v>
@@ -10389,7 +10398,7 @@
         <v>220</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G53" s="3">
         <v>64</v>
@@ -10413,7 +10422,7 @@
         <v>222</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G54" s="3">
         <v>65</v>
@@ -10437,7 +10446,7 @@
         <v>233</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="G55" s="3">
         <v>66</v>
@@ -10461,7 +10470,7 @@
         <v>234</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="G56" s="3">
         <v>67</v>
@@ -10485,7 +10494,7 @@
         <v>235</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G57" s="3">
         <v>68</v>
@@ -10506,10 +10515,10 @@
         <v>219</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>241</v>
+        <v>265</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>66</v>
+        <v>266</v>
       </c>
       <c r="G58" s="3">
         <v>69</v>
@@ -10530,10 +10539,10 @@
         <v>225</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>66</v>
+        <v>269</v>
       </c>
       <c r="G59" s="3">
         <v>70</v>

</xml_diff>

<commit_message>
Exemption Template file fix (#1315)
* migration issue

* sub type mismatch and data load fixes

* project loading issue

* work response fix

* project migration merge

* Exemption_Request template file fixes
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/exemption_request/001_Exemption_Request.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/exemption_request/001_Exemption_Request.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\eao\beta\code\epictrack-api\src\api\templates\event_templates\exemption_request\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E25389-8E21-435D-BE5D-E40194146CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC74BE90-31EE-4460-8EE8-9BB845619487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="274">
   <si>
     <t>No</t>
   </si>
@@ -940,9 +940,6 @@
     <t>Last Day of Exemption Request Readiness Decision (Date Capture Milestone)</t>
   </si>
   <si>
-    <t>Set workState to COMPLETE</t>
-  </si>
-  <si>
     <t>Set "Further Readiness Decision" PHASE to ACTIVE (show it)</t>
   </si>
   <si>
@@ -967,9 +964,6 @@
     <t>{"phase_name":"Exemption Early Engagement","work_type_id": 5, "ea_act_id": 3, "event_name": "Approval of IPD/EP Submission", "start_at": 1 }</t>
   </si>
   <si>
-    <t>{"phase_name":"Exemption Request Intake","work_type_id": 5, "ea_act_id": 3, "event_name": "Submission of "Draft" Initial Project Description &amp; Engagement Plan", "start_at": 21 }</t>
-  </si>
-  <si>
     <t>{"phase_name":"Exemption Request Intake","work_type_id": 5, "ea_act_id": 3, "event_name": "\"Draft\" Initial Project Description &amp; Engagement Plan Initial Review", "start_at": 28 }</t>
   </si>
   <si>
@@ -1028,6 +1022,21 @@
   </si>
   <si>
     <t>{"phase_name":"Further Readiness Decision","work_type_id": 5, "ea_act_id": 3, "event_name": "Readiness Decision Report referred to CEAO for Further Decision", "start_at": 1}</t>
+  </si>
+  <si>
+    <t>{"work_type": 6}</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Exemption DPD Development (Proponent Time)","work_type_id": 5, "ea_act_id": 3, "new_name": "Revised Exemption DPD Development (Proponent Time)", "legislated": false }</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Exemption Readiness Decision","work_type_id": 5, "ea_act_id": 3, "new_name": "Revised Exemption Readiness Decision", "legislated": false }</t>
+  </si>
+  <si>
+    <t>Exemption Order</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Exemption Request Intake","work_type_id": 5, "ea_act_id": 3, "event_name": "Submission of \"Draft\" Initial Project Description &amp; Engagement Plan", "start_at": 21 }</t>
   </si>
 </sst>
 </file>
@@ -1687,7 +1696,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1724,7 +1733,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -1738,7 +1747,7 @@
         <v>108</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>105</v>
+        <v>272</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>20</v>
@@ -1753,7 +1762,7 @@
         <v>65</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I2" s="3">
         <v>1</v>
@@ -1767,7 +1776,7 @@
         <v>109</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>105</v>
+        <v>272</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>20</v>
@@ -1782,7 +1791,7 @@
         <v>65</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I3" s="3">
         <v>2</v>
@@ -1796,7 +1805,7 @@
         <v>110</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>105</v>
+        <v>272</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>20</v>
@@ -1811,7 +1820,7 @@
         <v>65</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I4" s="3">
         <v>3</v>
@@ -1825,7 +1834,7 @@
         <v>111</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>105</v>
+        <v>272</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>20</v>
@@ -1840,7 +1849,7 @@
         <v>65</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I5" s="3">
         <v>4</v>
@@ -1854,7 +1863,7 @@
         <v>112</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>105</v>
+        <v>272</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>20</v>
@@ -1869,7 +1878,7 @@
         <v>65</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I6" s="3">
         <v>5</v>
@@ -1883,7 +1892,7 @@
         <v>113</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>105</v>
+        <v>272</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>20</v>
@@ -1898,7 +1907,7 @@
         <v>65</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="I7" s="3">
         <v>6</v>
@@ -2385,7 +2394,7 @@
   <dimension ref="A1:N126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="E65" sqref="E65"/>
@@ -2441,7 +2450,7 @@
         <v>4</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>7</v>
@@ -2480,7 +2489,7 @@
         <v>0</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N2" s="3">
         <v>1</v>
@@ -2519,7 +2528,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N3" s="3">
         <v>2</v>
@@ -2558,7 +2567,7 @@
         <v>0</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N4" s="3">
         <v>3</v>
@@ -2600,7 +2609,7 @@
         <v>0</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N5" s="3">
         <v>4</v>
@@ -2639,7 +2648,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N6" s="3">
         <v>5</v>
@@ -2678,7 +2687,7 @@
         <v>0</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N7" s="3">
         <v>6</v>
@@ -2720,7 +2729,7 @@
         <v>0</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N8" s="3">
         <v>7</v>
@@ -2762,7 +2771,7 @@
         <v>0</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N9" s="3">
         <v>8</v>
@@ -2801,7 +2810,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N10" s="3">
         <v>9</v>
@@ -2843,7 +2852,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N11" s="3">
         <v>10</v>
@@ -2882,7 +2891,7 @@
         <v>0</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N12" s="3">
         <v>11</v>
@@ -2921,7 +2930,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N13" s="3">
         <v>12</v>
@@ -2963,7 +2972,7 @@
         <v>0</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N14" s="3">
         <v>13</v>
@@ -3005,7 +3014,7 @@
         <v>0</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N15" s="3">
         <v>14</v>
@@ -3047,7 +3056,7 @@
         <v>0</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N16" s="3">
         <v>15</v>
@@ -3086,7 +3095,7 @@
         <v>0</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N17" s="3">
         <v>16</v>
@@ -3125,7 +3134,7 @@
         <v>30</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N18" s="3">
         <v>17</v>
@@ -3167,7 +3176,7 @@
         <v>0</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N19" s="3">
         <v>18</v>
@@ -3209,7 +3218,7 @@
         <v>0</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N20" s="3">
         <v>19</v>
@@ -3251,7 +3260,7 @@
         <v>0</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N21" s="3">
         <v>20</v>
@@ -3293,7 +3302,7 @@
         <v>0</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N22" s="3">
         <v>21</v>
@@ -3332,7 +3341,7 @@
         <v>0</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N23" s="3">
         <v>22</v>
@@ -3374,7 +3383,7 @@
         <v>0</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N24" s="3">
         <v>23</v>
@@ -3413,7 +3422,7 @@
         <v>0</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N25" s="3">
         <v>24</v>
@@ -3455,7 +3464,7 @@
         <v>0</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N26" s="3">
         <v>25</v>
@@ -3494,7 +3503,7 @@
         <v>0</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N27" s="3">
         <v>26</v>
@@ -3533,7 +3542,7 @@
         <v>0</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N28" s="3">
         <v>27</v>
@@ -3575,7 +3584,7 @@
         <v>0</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N29" s="3">
         <v>28</v>
@@ -3614,7 +3623,7 @@
         <v>0</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N30" s="3">
         <v>29</v>
@@ -3653,7 +3662,7 @@
         <v>0</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N31" s="3">
         <v>30</v>
@@ -3695,7 +3704,7 @@
         <v>0</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N32" s="3">
         <v>31</v>
@@ -3737,7 +3746,7 @@
         <v>0</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N33" s="3">
         <v>32</v>
@@ -3779,7 +3788,7 @@
         <v>0</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N34" s="3">
         <v>33</v>
@@ -3821,7 +3830,7 @@
         <v>0</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N35" s="3">
         <v>34</v>
@@ -3860,7 +3869,7 @@
         <v>30</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N36" s="3">
         <v>35</v>
@@ -3902,7 +3911,7 @@
         <v>0</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N37" s="3">
         <v>36</v>
@@ -3944,7 +3953,7 @@
         <v>0</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N38" s="3">
         <v>37</v>
@@ -3986,7 +3995,7 @@
         <v>0</v>
       </c>
       <c r="M39" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N39" s="3">
         <v>38</v>
@@ -4028,7 +4037,7 @@
         <v>0</v>
       </c>
       <c r="M40" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N40" s="3">
         <v>39</v>
@@ -4067,7 +4076,7 @@
         <v>0</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N41" s="3">
         <v>40</v>
@@ -4106,7 +4115,7 @@
         <v>0</v>
       </c>
       <c r="M42" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N42" s="3">
         <v>41</v>
@@ -4145,7 +4154,7 @@
         <v>0</v>
       </c>
       <c r="M43" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N43" s="3">
         <v>42</v>
@@ -4187,7 +4196,7 @@
         <v>0</v>
       </c>
       <c r="M44" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N44" s="3">
         <v>43</v>
@@ -4229,7 +4238,7 @@
         <v>0</v>
       </c>
       <c r="M45" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N45" s="3">
         <v>44</v>
@@ -4268,7 +4277,7 @@
         <v>0</v>
       </c>
       <c r="M46" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N46" s="3">
         <v>45</v>
@@ -4310,7 +4319,7 @@
         <v>0</v>
       </c>
       <c r="M47" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N47" s="3">
         <v>46</v>
@@ -4352,7 +4361,7 @@
         <v>0</v>
       </c>
       <c r="M48" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N48" s="3">
         <v>47</v>
@@ -4391,7 +4400,7 @@
         <v>0</v>
       </c>
       <c r="M49" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N49" s="3">
         <v>48</v>
@@ -4433,7 +4442,7 @@
         <v>0</v>
       </c>
       <c r="M50" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N50" s="3">
         <v>49</v>
@@ -4475,7 +4484,7 @@
         <v>0</v>
       </c>
       <c r="M51" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N51" s="3">
         <v>50</v>
@@ -4514,7 +4523,7 @@
         <v>0</v>
       </c>
       <c r="M52" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N52" s="3">
         <v>51</v>
@@ -4556,7 +4565,7 @@
         <v>0</v>
       </c>
       <c r="M53" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N53" s="3">
         <v>52</v>
@@ -4598,7 +4607,7 @@
         <v>0</v>
       </c>
       <c r="M54" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N54" s="3">
         <v>53</v>
@@ -4640,7 +4649,7 @@
         <v>0</v>
       </c>
       <c r="M55" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N55" s="3">
         <v>54</v>
@@ -4682,7 +4691,7 @@
         <v>0</v>
       </c>
       <c r="M56" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N56" s="3">
         <v>55</v>
@@ -4724,7 +4733,7 @@
         <v>0</v>
       </c>
       <c r="M57" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N57" s="3">
         <v>56</v>
@@ -4766,7 +4775,7 @@
         <v>0</v>
       </c>
       <c r="M58" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N58" s="3">
         <v>57</v>
@@ -4808,7 +4817,7 @@
         <v>0</v>
       </c>
       <c r="M59" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N59" s="3">
         <v>58</v>
@@ -4850,7 +4859,7 @@
         <v>0</v>
       </c>
       <c r="M60" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N60" s="3">
         <v>59</v>
@@ -4889,7 +4898,7 @@
         <v>0</v>
       </c>
       <c r="M61" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N61" s="3">
         <v>60</v>
@@ -4931,7 +4940,7 @@
         <v>0</v>
       </c>
       <c r="M62" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N62" s="3">
         <v>61</v>
@@ -4973,7 +4982,7 @@
         <v>0</v>
       </c>
       <c r="M63" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N63" s="3">
         <v>62</v>
@@ -5015,7 +5024,7 @@
         <v>0</v>
       </c>
       <c r="M64" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N64" s="3">
         <v>63</v>
@@ -5054,7 +5063,7 @@
         <v>0</v>
       </c>
       <c r="M65" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N65" s="3">
         <v>64</v>
@@ -5093,7 +5102,7 @@
         <v>0</v>
       </c>
       <c r="M66" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N66" s="3">
         <v>65</v>
@@ -5132,7 +5141,7 @@
         <v>0</v>
       </c>
       <c r="M67" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N67" s="3">
         <v>66</v>
@@ -5174,7 +5183,7 @@
         <v>0</v>
       </c>
       <c r="M68" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N68" s="3">
         <v>67</v>
@@ -5216,7 +5225,7 @@
         <v>0</v>
       </c>
       <c r="M69" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N69" s="3">
         <v>68</v>
@@ -5255,7 +5264,7 @@
         <v>0</v>
       </c>
       <c r="M70" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N70" s="3">
         <v>69</v>
@@ -5297,7 +5306,7 @@
         <v>0</v>
       </c>
       <c r="M71" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N71" s="3">
         <v>70</v>
@@ -5339,7 +5348,7 @@
         <v>0</v>
       </c>
       <c r="M72" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N72" s="3">
         <v>71</v>
@@ -5381,7 +5390,7 @@
         <v>0</v>
       </c>
       <c r="M73" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N73" s="3">
         <v>72</v>
@@ -5423,7 +5432,7 @@
         <v>0</v>
       </c>
       <c r="M74" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N74" s="3">
         <v>73</v>
@@ -5465,7 +5474,7 @@
         <v>0</v>
       </c>
       <c r="M75" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N75" s="3">
         <v>74</v>
@@ -5507,7 +5516,7 @@
         <v>0</v>
       </c>
       <c r="M76" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N76" s="3">
         <v>75</v>
@@ -5549,7 +5558,7 @@
         <v>0</v>
       </c>
       <c r="M77" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N77" s="3">
         <v>76</v>
@@ -5591,7 +5600,7 @@
         <v>0</v>
       </c>
       <c r="M78" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N78" s="3">
         <v>77</v>
@@ -5633,7 +5642,7 @@
         <v>0</v>
       </c>
       <c r="M79" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N79" s="3">
         <v>78</v>
@@ -5672,7 +5681,7 @@
         <v>0</v>
       </c>
       <c r="M80" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N80" s="3">
         <v>79</v>
@@ -5711,7 +5720,7 @@
         <v>0</v>
       </c>
       <c r="M81" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N81" s="3">
         <v>80</v>
@@ -5750,7 +5759,7 @@
         <v>0</v>
       </c>
       <c r="M82" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N82" s="3">
         <v>81</v>
@@ -5792,7 +5801,7 @@
         <v>0</v>
       </c>
       <c r="M83" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N83" s="3">
         <v>82</v>
@@ -5834,7 +5843,7 @@
         <v>0</v>
       </c>
       <c r="M84" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N84" s="3">
         <v>83</v>
@@ -5873,7 +5882,7 @@
         <v>0</v>
       </c>
       <c r="M85" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N85" s="3">
         <v>84</v>
@@ -5912,7 +5921,7 @@
         <v>0</v>
       </c>
       <c r="M86" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N86" s="3">
         <v>85</v>
@@ -5954,7 +5963,7 @@
         <v>0</v>
       </c>
       <c r="M87" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N87" s="3">
         <v>86</v>
@@ -5996,7 +6005,7 @@
         <v>0</v>
       </c>
       <c r="M88" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N88" s="3">
         <v>87</v>
@@ -6038,7 +6047,7 @@
         <v>0</v>
       </c>
       <c r="M89" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N89" s="3">
         <v>88</v>
@@ -6080,7 +6089,7 @@
         <v>0</v>
       </c>
       <c r="M90" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N90" s="3">
         <v>89</v>
@@ -6119,7 +6128,7 @@
         <v>0</v>
       </c>
       <c r="M91" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N91" s="3">
         <v>90</v>
@@ -6158,7 +6167,7 @@
         <v>0</v>
       </c>
       <c r="M92" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N92" s="3">
         <v>91</v>
@@ -6200,7 +6209,7 @@
         <v>0</v>
       </c>
       <c r="M93" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N93" s="3">
         <v>92</v>
@@ -6242,7 +6251,7 @@
         <v>0</v>
       </c>
       <c r="M94" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N94" s="3">
         <v>93</v>
@@ -6284,7 +6293,7 @@
         <v>0</v>
       </c>
       <c r="M95" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N95" s="3">
         <v>94</v>
@@ -6326,7 +6335,7 @@
         <v>0</v>
       </c>
       <c r="M96" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N96" s="3">
         <v>95</v>
@@ -6368,7 +6377,7 @@
         <v>0</v>
       </c>
       <c r="M97" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N97" s="3">
         <v>96</v>
@@ -6410,7 +6419,7 @@
         <v>0</v>
       </c>
       <c r="M98" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N98" s="3">
         <v>97</v>
@@ -6452,7 +6461,7 @@
         <v>0</v>
       </c>
       <c r="M99" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N99" s="3">
         <v>98</v>
@@ -6494,7 +6503,7 @@
         <v>0</v>
       </c>
       <c r="M100" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N100" s="3">
         <v>99</v>
@@ -6536,7 +6545,7 @@
         <v>0</v>
       </c>
       <c r="M101" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N101" s="3">
         <v>100</v>
@@ -6575,7 +6584,7 @@
         <v>0</v>
       </c>
       <c r="M102" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N102" s="3">
         <v>101</v>
@@ -6614,7 +6623,7 @@
         <v>0</v>
       </c>
       <c r="M103" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N103" s="3">
         <v>102</v>
@@ -6653,7 +6662,7 @@
         <v>0</v>
       </c>
       <c r="M104" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N104" s="3">
         <v>103</v>
@@ -6692,7 +6701,7 @@
         <v>0</v>
       </c>
       <c r="M105" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N105" s="3">
         <v>104</v>
@@ -6734,7 +6743,7 @@
         <v>0</v>
       </c>
       <c r="M106" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N106" s="3">
         <v>105</v>
@@ -6776,7 +6785,7 @@
         <v>0</v>
       </c>
       <c r="M107" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N107" s="3">
         <v>106</v>
@@ -6818,7 +6827,7 @@
         <v>0</v>
       </c>
       <c r="M108" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N108" s="3">
         <v>107</v>
@@ -6860,7 +6869,7 @@
         <v>0</v>
       </c>
       <c r="M109" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N109" s="3">
         <v>108</v>
@@ -6902,7 +6911,7 @@
         <v>0</v>
       </c>
       <c r="M110" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N110" s="3">
         <v>109</v>
@@ -6944,7 +6953,7 @@
         <v>0</v>
       </c>
       <c r="M111" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N111" s="3">
         <v>110</v>
@@ -6983,7 +6992,7 @@
         <v>0</v>
       </c>
       <c r="M112" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N112" s="3">
         <v>111</v>
@@ -7025,7 +7034,7 @@
         <v>0</v>
       </c>
       <c r="M113" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N113" s="3">
         <v>112</v>
@@ -7067,7 +7076,7 @@
         <v>0</v>
       </c>
       <c r="M114" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N114" s="3">
         <v>113</v>
@@ -7106,7 +7115,7 @@
         <v>0</v>
       </c>
       <c r="M115" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N115" s="3">
         <v>114</v>
@@ -7145,7 +7154,7 @@
         <v>0</v>
       </c>
       <c r="M116" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N116" s="3">
         <v>115</v>
@@ -7187,7 +7196,7 @@
         <v>0</v>
       </c>
       <c r="M117" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N117" s="3">
         <v>116</v>
@@ -7229,7 +7238,7 @@
         <v>0</v>
       </c>
       <c r="M118" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N118" s="3">
         <v>117</v>
@@ -7271,7 +7280,7 @@
         <v>0</v>
       </c>
       <c r="M119" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N119" s="3">
         <v>118</v>
@@ -7313,7 +7322,7 @@
         <v>0</v>
       </c>
       <c r="M120" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N120" s="3">
         <v>119</v>
@@ -7355,7 +7364,7 @@
         <v>0</v>
       </c>
       <c r="M121" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N121" s="3">
         <v>120</v>
@@ -7397,7 +7406,7 @@
         <v>0</v>
       </c>
       <c r="M122" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N122" s="3">
         <v>121</v>
@@ -7436,7 +7445,7 @@
         <v>0</v>
       </c>
       <c r="M123" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N123" s="3">
         <v>122</v>
@@ -7478,7 +7487,7 @@
         <v>0</v>
       </c>
       <c r="M124" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N124" s="3">
         <v>123</v>
@@ -7520,7 +7529,7 @@
         <v>0</v>
       </c>
       <c r="M125" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N125" s="3">
         <v>124</v>
@@ -7562,7 +7571,7 @@
         <v>0</v>
       </c>
       <c r="M126" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N126" s="3">
         <v>125</v>
@@ -9106,10 +9115,10 @@
   <dimension ref="A1:G59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E48" sqref="E48"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9165,7 +9174,7 @@
         <v>211</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G2" s="3">
         <v>1</v>
@@ -9189,7 +9198,7 @@
         <v>213</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>250</v>
+        <v>273</v>
       </c>
       <c r="G3" s="3">
         <v>2</v>
@@ -9213,7 +9222,7 @@
         <v>214</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G4" s="3">
         <v>3</v>
@@ -9237,7 +9246,7 @@
         <v>216</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G5" s="3">
         <v>4</v>
@@ -9261,7 +9270,7 @@
         <v>220</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G6" s="3">
         <v>6</v>
@@ -9285,7 +9294,7 @@
         <v>222</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G7" s="3">
         <v>7</v>
@@ -9309,7 +9318,7 @@
         <v>224</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="G8" s="3">
         <v>8</v>
@@ -9333,7 +9342,7 @@
         <v>226</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G9" s="3">
         <v>9</v>
@@ -9357,7 +9366,7 @@
         <v>216</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G10" s="3">
         <v>10</v>
@@ -9381,7 +9390,7 @@
         <v>227</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G11" s="3">
         <v>12</v>
@@ -9405,7 +9414,7 @@
         <v>222</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G12" s="3">
         <v>13</v>
@@ -9429,7 +9438,7 @@
         <v>216</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G13" s="3">
         <v>14</v>
@@ -9453,7 +9462,7 @@
         <v>220</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G14" s="3">
         <v>16</v>
@@ -9477,7 +9486,7 @@
         <v>222</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G15" s="3">
         <v>17</v>
@@ -9501,7 +9510,7 @@
         <v>228</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="G16" s="3">
         <v>18</v>
@@ -9525,7 +9534,7 @@
         <v>229</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G17" s="3">
         <v>19</v>
@@ -9549,7 +9558,7 @@
         <v>230</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G18" s="3">
         <v>20</v>
@@ -9573,7 +9582,7 @@
         <v>231</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G19" s="3">
         <v>21</v>
@@ -9597,7 +9606,7 @@
         <v>226</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G20" s="3">
         <v>22</v>
@@ -9621,7 +9630,7 @@
         <v>216</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G21" s="3">
         <v>23</v>
@@ -9645,7 +9654,7 @@
         <v>227</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G22" s="3">
         <v>25</v>
@@ -9669,7 +9678,7 @@
         <v>222</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G23" s="3">
         <v>26</v>
@@ -9693,7 +9702,7 @@
         <v>216</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G24" s="3">
         <v>27</v>
@@ -9717,7 +9726,7 @@
         <v>220</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G25" s="3">
         <v>29</v>
@@ -9741,7 +9750,7 @@
         <v>222</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G26" s="3">
         <v>30</v>
@@ -9765,7 +9774,7 @@
         <v>218</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G27" s="3">
         <v>31</v>
@@ -9789,7 +9798,7 @@
         <v>237</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G28" s="3">
         <v>32</v>
@@ -9813,7 +9822,7 @@
         <v>233</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G29" s="3">
         <v>33</v>
@@ -9837,7 +9846,7 @@
         <v>234</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G30" s="3">
         <v>34</v>
@@ -9861,7 +9870,7 @@
         <v>235</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G31" s="3">
         <v>35</v>
@@ -9885,7 +9894,7 @@
         <v>226</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G32" s="3">
         <v>37</v>
@@ -9909,7 +9918,7 @@
         <v>216</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G33" s="3">
         <v>38</v>
@@ -9933,7 +9942,7 @@
         <v>227</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G34" s="3">
         <v>40</v>
@@ -9957,7 +9966,7 @@
         <v>222</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G35" s="3">
         <v>41</v>
@@ -9981,7 +9990,7 @@
         <v>216</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G36" s="3">
         <v>42</v>
@@ -10005,7 +10014,7 @@
         <v>220</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G37" s="3">
         <v>44</v>
@@ -10029,7 +10038,7 @@
         <v>222</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G38" s="3">
         <v>45</v>
@@ -10053,7 +10062,7 @@
         <v>216</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G39" s="3">
         <v>46</v>
@@ -10077,7 +10086,7 @@
         <v>227</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G40" s="3">
         <v>48</v>
@@ -10101,7 +10110,7 @@
         <v>222</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G41" s="3">
         <v>49</v>
@@ -10125,7 +10134,7 @@
         <v>216</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G42" s="3">
         <v>50</v>
@@ -10149,7 +10158,7 @@
         <v>220</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G43" s="3">
         <v>52</v>
@@ -10173,7 +10182,7 @@
         <v>222</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G44" s="3">
         <v>53</v>
@@ -10194,10 +10203,10 @@
         <v>219</v>
       </c>
       <c r="E45" s="29" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G45" s="3">
         <v>54</v>
@@ -10221,7 +10230,7 @@
         <v>222</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G46" s="3">
         <v>55</v>
@@ -10242,10 +10251,10 @@
         <v>232</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G47" s="3">
         <v>56</v>
@@ -10266,10 +10275,10 @@
         <v>210</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G48" s="3">
         <v>57</v>
@@ -10293,7 +10302,7 @@
         <v>216</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G49" s="3">
         <v>58</v>
@@ -10317,7 +10326,7 @@
         <v>227</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G50" s="3">
         <v>60</v>
@@ -10341,7 +10350,7 @@
         <v>222</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G51" s="3">
         <v>61</v>
@@ -10365,7 +10374,7 @@
         <v>216</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G52" s="3">
         <v>62</v>
@@ -10389,7 +10398,7 @@
         <v>220</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G53" s="3">
         <v>64</v>
@@ -10413,7 +10422,7 @@
         <v>222</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G54" s="3">
         <v>65</v>
@@ -10437,7 +10446,7 @@
         <v>233</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="G55" s="3">
         <v>66</v>
@@ -10461,7 +10470,7 @@
         <v>234</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="G56" s="3">
         <v>67</v>
@@ -10485,7 +10494,7 @@
         <v>235</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G57" s="3">
         <v>68</v>
@@ -10506,10 +10515,10 @@
         <v>219</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>241</v>
+        <v>265</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>66</v>
+        <v>266</v>
       </c>
       <c r="G58" s="3">
         <v>69</v>
@@ -10530,10 +10539,10 @@
         <v>225</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>66</v>
+        <v>269</v>
       </c>
       <c r="G59" s="3">
         <v>70</v>

</xml_diff>